<commit_message>
Updated Excell files. Made a new copy of database jupyter notebook.
</commit_message>
<xml_diff>
--- a/Jupyter/Eurofer/Eurofer_data.xlsx
+++ b/Jupyter/Eurofer/Eurofer_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Research\Repos\ZapRepo\Computer Codes\Jupyter\Eurofer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Research\Repos\DatabaseCodes\Jupyter\Eurofer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29790B9F-C8C3-489E-8BF3-44465D10EBF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B7EB94-3307-482C-B730-12F2EDA47712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="852" activeTab="2" xr2:uid="{D289EE42-B074-4616-9B9B-4CE9F1662138}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="852" activeTab="3" xr2:uid="{D289EE42-B074-4616-9B9B-4CE9F1662138}"/>
   </bookViews>
   <sheets>
     <sheet name="Eurofer_density" sheetId="15" r:id="rId1"/>
@@ -53,9 +53,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="87">
   <si>
     <t>Temp (K)</t>
-  </si>
-  <si>
-    <t>Thermal Conductivity, k (W/m-K)</t>
   </si>
   <si>
     <r>
@@ -333,9 +330,6 @@
     <t>Temp ( C )</t>
   </si>
   <si>
-    <t>ThermalConductivity (W/mK)</t>
-  </si>
-  <si>
     <t>EUROFER97-Sy</t>
   </si>
   <si>
@@ -601,6 +595,12 @@
   </si>
   <si>
     <t>SpecificHeat (J_kg-K)</t>
+  </si>
+  <si>
+    <t>ThermalConductivity (W_mK)</t>
+  </si>
+  <si>
+    <t>Thermal Conductivity, k (W_m-K)</t>
   </si>
 </sst>
 </file>
@@ -1330,15 +1330,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>26609</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>71059</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>171046</xdr:rowOff>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>215496</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1367,8 +1367,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="19050" y="3646109"/>
-          <a:ext cx="3384550" cy="2620937"/>
+          <a:off x="0" y="3938209"/>
+          <a:ext cx="3536950" cy="2538387"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1380,15 +1380,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>717550</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>276849</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>118099</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>248081</xdr:rowOff>
+      <xdr:rowOff>2470581</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1411,8 +1411,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4191000" y="3638550"/>
-          <a:ext cx="4467849" cy="3086531"/>
+          <a:off x="5099050" y="5740400"/>
+          <a:ext cx="4658349" cy="2991281"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2394,7 +2394,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -2402,7 +2402,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -2491,15 +2491,15 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -2525,66 +2525,66 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="16"/>
       <c r="D1" s="16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E1" s="16"/>
       <c r="G1" s="16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H1" s="16"/>
       <c r="J1" s="16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K1" s="16"/>
       <c r="P1" s="16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="Q1" s="16"/>
       <c r="S1" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="T1" s="16"/>
     </row>
     <row r="3" spans="1:20" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="G3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="S3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.35">
@@ -2607,19 +2607,19 @@
         <v>634.60653000000002</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K4" s="2">
         <v>682.89473684210498</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="Q4" s="2">
         <v>886</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="T4" s="2">
         <v>1066</v>
@@ -2985,21 +2985,21 @@
     </row>
     <row r="39" spans="1:20" ht="152.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B39" s="16"/>
       <c r="E39" s="16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F39" s="16"/>
       <c r="G39" s="16"/>
       <c r="H39" s="16"/>
       <c r="J39" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K39" s="16"/>
       <c r="P39" s="16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="Q39" s="16"/>
       <c r="R39" s="16"/>
@@ -3008,7 +3008,7 @@
     </row>
     <row r="40" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -3047,24 +3047,24 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="15"/>
       <c r="E1" s="2"/>
       <c r="F1" s="15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G1" s="15"/>
       <c r="H1" s="15"/>
       <c r="I1" s="15"/>
       <c r="K1" s="15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L1" s="15"/>
       <c r="M1" s="15"/>
       <c r="N1" s="15"/>
       <c r="P1" s="15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q1" s="15"/>
       <c r="R1" s="15"/>
@@ -3072,49 +3072,49 @@
     </row>
     <row r="3" spans="1:20" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="6"/>
       <c r="F3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.35">
@@ -3525,13 +3525,13 @@
     </row>
     <row r="41" spans="1:20" ht="84.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B41" s="16"/>
       <c r="C41" s="16"/>
       <c r="D41" s="16"/>
       <c r="F41" s="15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G41" s="15"/>
       <c r="H41" s="15"/>
@@ -3550,7 +3550,7 @@
     </row>
     <row r="42" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B42" s="20"/>
       <c r="C42" s="7"/>
@@ -3617,56 +3617,56 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B1" s="16"/>
       <c r="D1" s="16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E1" s="16"/>
       <c r="G1" s="16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H1" s="16"/>
       <c r="J1" s="16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K1" s="16"/>
       <c r="M1" s="16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="N1" s="16"/>
     </row>
     <row r="3" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="D3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="G3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="J3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="M3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="N3" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
@@ -4004,7 +4004,7 @@
     </row>
     <row r="34" spans="1:23" ht="147" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B34" s="16"/>
       <c r="C34" s="16"/>
@@ -4017,7 +4017,7 @@
       <c r="J34" s="16"/>
       <c r="K34" s="16"/>
       <c r="M34" s="16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="N34" s="16"/>
       <c r="O34" s="11"/>
@@ -4074,76 +4074,76 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B1" s="16"/>
       <c r="D1" s="16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E1" s="16"/>
       <c r="G1" s="16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H1" s="16"/>
       <c r="J1" s="16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K1" s="16"/>
       <c r="M1" s="16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="N1" s="16"/>
       <c r="P1" s="16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="Q1" s="16"/>
       <c r="S1" s="16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="T1" s="16"/>
     </row>
     <row r="3" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.35">
@@ -4876,14 +4876,14 @@
     </row>
     <row r="39" spans="1:17" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B39" s="16"/>
       <c r="C39" s="16"/>
       <c r="D39" s="16"/>
       <c r="E39" s="16"/>
       <c r="G39" s="16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H39" s="16"/>
       <c r="I39" s="16"/>
@@ -4895,7 +4895,7 @@
     </row>
     <row r="52" spans="16:20" ht="93.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="P52" s="16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="Q52" s="16"/>
       <c r="R52" s="16"/>
@@ -4950,7 +4950,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="15"/>
       <c r="D1" s="15"/>
@@ -4967,7 +4967,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E3" s="2"/>
     </row>
@@ -5037,13 +5037,13 @@
     </row>
     <row r="36" spans="1:2" ht="156" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B36" s="16"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -5065,7 +5065,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{234A6B1F-5943-445E-8C13-06397E85A588}">
   <dimension ref="A1:Y49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
@@ -5077,11 +5077,11 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="16"/>
       <c r="D1" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E1" s="16"/>
     </row>
@@ -5090,13 +5090,13 @@
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -5107,7 +5107,7 @@
         <v>448.39537869062798</v>
       </c>
       <c r="D4" s="2">
-        <f>I32+273</f>
+        <f t="shared" ref="D4:D18" si="0">I32+273</f>
         <v>293.54795000000001</v>
       </c>
       <c r="E4" s="2">
@@ -5122,7 +5122,7 @@
         <v>461.48908857509599</v>
       </c>
       <c r="D5" s="2">
-        <f>I33+273</f>
+        <f t="shared" si="0"/>
         <v>326.42466000000002</v>
       </c>
       <c r="E5" s="2">
@@ -5137,7 +5137,7 @@
         <v>475.35301668806102</v>
       </c>
       <c r="D6" s="2">
-        <f>I34+273</f>
+        <f t="shared" si="0"/>
         <v>373</v>
       </c>
       <c r="E6" s="2">
@@ -5152,7 +5152,7 @@
         <v>485.36585365853603</v>
       </c>
       <c r="D7" s="2">
-        <f>I35+273</f>
+        <f t="shared" si="0"/>
         <v>425.05479000000003</v>
       </c>
       <c r="E7" s="2">
@@ -5167,7 +5167,7 @@
         <v>496.14890885750901</v>
       </c>
       <c r="D8" s="2">
-        <f>I36+273</f>
+        <f t="shared" si="0"/>
         <v>474.36986000000002</v>
       </c>
       <c r="E8" s="2">
@@ -5182,7 +5182,7 @@
         <v>504.621309370988</v>
       </c>
       <c r="D9" s="2">
-        <f>I37+273</f>
+        <f t="shared" si="0"/>
         <v>523.68493000000001</v>
       </c>
       <c r="E9" s="2">
@@ -5197,7 +5197,7 @@
         <v>513.86392811296503</v>
       </c>
       <c r="D10" s="2">
-        <f>I38+273</f>
+        <f t="shared" si="0"/>
         <v>573</v>
       </c>
       <c r="E10" s="2">
@@ -5212,7 +5212,7 @@
         <v>521.56611039794598</v>
       </c>
       <c r="D11" s="2">
-        <f>I39+273</f>
+        <f t="shared" si="0"/>
         <v>622.31506999999999</v>
       </c>
       <c r="E11" s="2">
@@ -5227,7 +5227,7 @@
         <v>530.03851091142405</v>
       </c>
       <c r="D12" s="2">
-        <f>I40+273</f>
+        <f t="shared" si="0"/>
         <v>671.63013999999998</v>
       </c>
       <c r="E12" s="2">
@@ -5242,7 +5242,7 @@
         <v>536.97047496790697</v>
       </c>
       <c r="D13" s="2">
-        <f>I41+273</f>
+        <f t="shared" si="0"/>
         <v>723.68493000000001</v>
       </c>
       <c r="E13" s="2">
@@ -5257,7 +5257,7 @@
         <v>544.67265725288803</v>
       </c>
       <c r="D14" s="2">
-        <f>I42+273</f>
+        <f t="shared" si="0"/>
         <v>773</v>
       </c>
       <c r="E14" s="2">
@@ -5272,7 +5272,7 @@
         <v>550.83440308087199</v>
       </c>
       <c r="D15" s="2">
-        <f>I43+273</f>
+        <f t="shared" si="0"/>
         <v>822.31506999999999</v>
       </c>
       <c r="E15" s="2">
@@ -5287,7 +5287,7 @@
         <v>556.99614890885698</v>
       </c>
       <c r="D16" s="2">
-        <f>I44+273</f>
+        <f t="shared" si="0"/>
         <v>871.63013999999998</v>
       </c>
       <c r="E16" s="2">
@@ -5302,7 +5302,7 @@
         <v>565.46854942233597</v>
       </c>
       <c r="D17" s="2">
-        <f>I45+273</f>
+        <f t="shared" si="0"/>
         <v>920.94520999999997</v>
       </c>
       <c r="E17" s="2">
@@ -5317,7 +5317,7 @@
         <v>573.17073170731703</v>
       </c>
       <c r="D18" s="2">
-        <f>I46+273</f>
+        <f t="shared" si="0"/>
         <v>973</v>
       </c>
       <c r="E18" s="2">
@@ -5398,7 +5398,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I31" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
@@ -5479,17 +5479,17 @@
     </row>
     <row r="47" spans="1:25" ht="285" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B47" s="16"/>
       <c r="D47" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E47" s="16"/>
     </row>
     <row r="49" spans="1:1" ht="29" x14ac:dyDescent="0.35">
       <c r="A49" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -5511,8 +5511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D45C8D-0E1D-4271-9C84-7C91BB3EB92B}">
   <dimension ref="A1:V39"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5523,11 +5523,11 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="16"/>
       <c r="D1" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E1" s="16"/>
     </row>
@@ -5536,13 +5536,13 @@
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>1</v>
+        <v>86</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -5699,17 +5699,17 @@
     </row>
     <row r="33" spans="1:22" ht="208.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B33" s="16"/>
       <c r="D33" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E33" s="16"/>
     </row>
     <row r="35" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.35">
@@ -5750,7 +5750,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="15"/>
       <c r="D1" s="15"/>
@@ -5767,7 +5767,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="2"/>
@@ -5961,13 +5961,13 @@
     </row>
     <row r="53" spans="1:2" ht="210" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B53" s="16"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -5999,16 +5999,16 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="16"/>
     </row>
     <row r="3" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -6069,13 +6069,13 @@
     </row>
     <row r="39" spans="1:2" ht="187.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B39" s="16"/>
     </row>
     <row r="40" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -6106,15 +6106,15 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="16"/>
       <c r="D1" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E1" s="16"/>
       <c r="G1" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H1" s="16"/>
       <c r="I1" s="16"/>
@@ -6124,22 +6124,22 @@
         <v>0</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -6278,12 +6278,12 @@
     </row>
     <row r="33" spans="1:14" ht="153" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B33" s="17"/>
       <c r="C33" s="9"/>
       <c r="D33" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E33" s="17"/>
       <c r="F33" s="17"/>
@@ -6292,7 +6292,7 @@
       <c r="I33" s="17"/>
       <c r="J33" s="9"/>
       <c r="K33" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L33" s="17"/>
       <c r="M33" s="17"/>
@@ -6300,7 +6300,7 @@
     </row>
     <row r="34" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A34" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -6336,16 +6336,16 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B1" s="18"/>
     </row>
     <row r="3" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -6422,7 +6422,7 @@
     </row>
     <row r="27" spans="1:2" ht="179.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B27" s="16"/>
     </row>
@@ -6458,64 +6458,64 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B1" s="19"/>
       <c r="D1" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E1" s="19"/>
       <c r="G1" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H1" s="19"/>
       <c r="J1" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K1" s="19"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="19" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B2" s="19"/>
       <c r="D2" s="19" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E2" s="19"/>
       <c r="G2" s="19" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H2" s="19"/>
       <c r="J2" s="19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K2" s="19"/>
     </row>
     <row r="3" spans="1:11" ht="33.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
@@ -6784,7 +6784,7 @@
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" s="16" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
fixed all programs to produce a simple script in each cell.
</commit_message>
<xml_diff>
--- a/Jupyter/Eurofer/Eurofer_data.xlsx
+++ b/Jupyter/Eurofer/Eurofer_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fuqih\Documents\GitHub\DatabaseCodes\Jupyter\Eurofer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Research\Repos\DatabaseCodes\Jupyter\Eurofer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164CF13F-AB21-4EC6-BF35-C97E57DB78C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE03CF13-0199-4EF8-8DB8-7B60A609EBEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="852" xr2:uid="{D289EE42-B074-4616-9B9B-4CE9F1662138}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="852" activeTab="3" xr2:uid="{D289EE42-B074-4616-9B9B-4CE9F1662138}"/>
   </bookViews>
   <sheets>
     <sheet name="Eurofer_density" sheetId="15" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="101">
   <si>
     <t>Temp (K)</t>
   </si>
@@ -617,6 +617,9 @@
   </si>
   <si>
     <t>EUROFER97 E83699 1075 °C + 750 °C + 600 °C 1050h</t>
+  </si>
+  <si>
+    <t>Temp(K)</t>
   </si>
 </sst>
 </file>
@@ -2488,22 +2491,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10AFBB79-7160-4576-990E-E539762E50F4}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H14" sqref="H14:H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="16"/>
     </row>
-    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -2511,7 +2514,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>293</v>
       </c>
@@ -2519,7 +2522,7 @@
         <v>7750</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>373</v>
       </c>
@@ -2527,7 +2530,7 @@
         <v>7728</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>473</v>
       </c>
@@ -2535,7 +2538,7 @@
         <v>7699</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>573</v>
       </c>
@@ -2543,7 +2546,7 @@
         <v>7666</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>673</v>
       </c>
@@ -2551,7 +2554,7 @@
         <v>7633</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>773</v>
       </c>
@@ -2559,7 +2562,7 @@
         <v>7596</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>873</v>
       </c>
@@ -2583,64 +2586,64 @@
       <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="12.5703125" style="2"/>
-    <col min="3" max="3" width="12.5703125" style="2" customWidth="1"/>
-    <col min="4" max="9" width="12.5703125" style="2"/>
-    <col min="10" max="14" width="12.85546875" style="2" customWidth="1"/>
-    <col min="15" max="15" width="12.5703125" style="2"/>
-    <col min="16" max="16" width="5.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="2.42578125" style="2" customWidth="1"/>
-    <col min="19" max="19" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="3.5703125" style="2" customWidth="1"/>
-    <col min="22" max="22" width="5.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="2.85546875" style="2" customWidth="1"/>
-    <col min="25" max="25" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="3.5703125" style="2" customWidth="1"/>
-    <col min="28" max="28" width="5.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="12.54296875" style="2"/>
+    <col min="3" max="3" width="12.54296875" style="2" customWidth="1"/>
+    <col min="4" max="9" width="12.54296875" style="2"/>
+    <col min="10" max="14" width="12.81640625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="12.54296875" style="2"/>
+    <col min="16" max="16" width="5.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="2.453125" style="2" customWidth="1"/>
+    <col min="19" max="19" width="5.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="3.54296875" style="2" customWidth="1"/>
+    <col min="22" max="22" width="5.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="2.81640625" style="2" customWidth="1"/>
+    <col min="25" max="25" width="5.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="3.54296875" style="2" customWidth="1"/>
+    <col min="28" max="28" width="5.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="3" style="2" customWidth="1"/>
-    <col min="31" max="31" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="3.5703125" style="2" customWidth="1"/>
-    <col min="34" max="34" width="5.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="8.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="3.42578125" style="2" customWidth="1"/>
-    <col min="37" max="37" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="8.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="3.5703125" style="2" customWidth="1"/>
-    <col min="40" max="40" width="5.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="8.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="3.28515625" style="2" customWidth="1"/>
-    <col min="43" max="43" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="8.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="3.5703125" style="2" customWidth="1"/>
-    <col min="46" max="46" width="5.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="8.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="2.140625" style="2" customWidth="1"/>
-    <col min="49" max="49" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="8.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="3.5703125" style="2" customWidth="1"/>
-    <col min="52" max="52" width="5.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="8.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="5.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="3.54296875" style="2" customWidth="1"/>
+    <col min="34" max="34" width="5.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="3.453125" style="2" customWidth="1"/>
+    <col min="37" max="37" width="5.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="3.54296875" style="2" customWidth="1"/>
+    <col min="40" max="40" width="5.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="3.26953125" style="2" customWidth="1"/>
+    <col min="43" max="43" width="5.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="3.54296875" style="2" customWidth="1"/>
+    <col min="46" max="46" width="5.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="2.1796875" style="2" customWidth="1"/>
+    <col min="49" max="49" width="5.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="3.54296875" style="2" customWidth="1"/>
+    <col min="52" max="52" width="5.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="5" style="2" customWidth="1"/>
-    <col min="55" max="55" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="8.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="3.5703125" style="2" customWidth="1"/>
-    <col min="58" max="58" width="5.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="8.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="3.140625" style="2" customWidth="1"/>
-    <col min="61" max="61" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="8.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="63" max="16384" width="12.5703125" style="2"/>
+    <col min="55" max="55" width="5.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="3.54296875" style="2" customWidth="1"/>
+    <col min="58" max="58" width="5.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="3.1796875" style="2" customWidth="1"/>
+    <col min="61" max="61" width="5.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="63" max="16384" width="12.54296875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:62" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>11</v>
       </c>
@@ -2734,8 +2737,8 @@
       </c>
       <c r="BJ1" s="16"/>
     </row>
-    <row r="2" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:62" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:62" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -2863,7 +2866,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>20</v>
       </c>
@@ -3006,7 +3009,7 @@
         <v>621.67832167832103</v>
       </c>
     </row>
-    <row r="5" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>50</v>
       </c>
@@ -3149,7 +3152,7 @@
         <v>505.233380480905</v>
       </c>
     </row>
-    <row r="6" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>100</v>
       </c>
@@ -3292,7 +3295,7 @@
         <v>475.53041018387501</v>
       </c>
     </row>
-    <row r="7" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>150</v>
       </c>
@@ -3427,7 +3430,7 @@
         <v>399.15134370579898</v>
       </c>
     </row>
-    <row r="8" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>200</v>
       </c>
@@ -3562,7 +3565,7 @@
         <v>282.46110325318199</v>
       </c>
     </row>
-    <row r="9" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>250</v>
       </c>
@@ -3649,7 +3652,7 @@
       <c r="BI9" s="15"/>
       <c r="BJ9" s="15"/>
     </row>
-    <row r="10" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>300</v>
       </c>
@@ -3669,7 +3672,7 @@
         <v>495.42626000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>350</v>
       </c>
@@ -3689,7 +3692,7 @@
         <v>466.57317999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>400</v>
       </c>
@@ -3709,7 +3712,7 @@
         <v>432.49275</v>
       </c>
     </row>
-    <row r="13" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>450</v>
       </c>
@@ -3729,7 +3732,7 @@
         <v>389.26197000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>500</v>
       </c>
@@ -3749,7 +3752,7 @@
         <v>339.49808999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>550</v>
       </c>
@@ -3769,7 +3772,7 @@
         <v>276.65652999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>600</v>
       </c>
@@ -3789,7 +3792,7 @@
         <v>199.44013000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>650</v>
       </c>
@@ -3809,7 +3812,7 @@
         <v>105.22734</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>700</v>
       </c>
@@ -3817,7 +3820,7 @@
         <v>137.14859437750999</v>
       </c>
     </row>
-    <row r="39" spans="1:62" ht="152.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:62" ht="152.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="16" t="s">
         <v>17</v>
       </c>
@@ -3885,13 +3888,22 @@
       <c r="BI39" s="16"/>
       <c r="BJ39" s="16"/>
     </row>
-    <row r="40" spans="1:62" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:62" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" s="7" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="BF1:BG1"/>
+    <mergeCell ref="BI1:BJ1"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="J39:N39"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:H1"/>
     <mergeCell ref="P39:BJ39"/>
     <mergeCell ref="E39:H39"/>
     <mergeCell ref="P1:Q1"/>
@@ -3905,18 +3917,9 @@
     <mergeCell ref="AN1:AO1"/>
     <mergeCell ref="AQ1:AR1"/>
     <mergeCell ref="AT1:AU1"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="J39:N39"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="G1:H1"/>
     <mergeCell ref="AW1:AX1"/>
     <mergeCell ref="AZ1:BA1"/>
     <mergeCell ref="BC1:BD1"/>
-    <mergeCell ref="BF1:BG1"/>
-    <mergeCell ref="BI1:BJ1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A40" r:id="rId1" xr:uid="{BD8505B1-6312-437D-81B2-778CAED7521D}"/>
@@ -3934,12 +3937,12 @@
       <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="12.5703125" style="1"/>
+    <col min="1" max="16384" width="12.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>11</v>
       </c>
@@ -3972,7 +3975,7 @@
       </c>
       <c r="T1" s="17"/>
     </row>
-    <row r="3" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -4020,7 +4023,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>20</v>
       </c>
@@ -4068,7 +4071,7 @@
         <v>7.3191884470258204</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>50</v>
       </c>
@@ -4116,7 +4119,7 @@
         <v>9.1572334498903505</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>100</v>
       </c>
@@ -4165,7 +4168,7 @@
       </c>
       <c r="U6" s="10"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>150</v>
       </c>
@@ -4214,7 +4217,7 @@
       </c>
       <c r="U7" s="10"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>200</v>
       </c>
@@ -4253,7 +4256,7 @@
       <c r="T8" s="10"/>
       <c r="U8" s="10"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>250</v>
       </c>
@@ -4292,7 +4295,7 @@
       <c r="T9" s="10"/>
       <c r="U9" s="10"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>300</v>
       </c>
@@ -4324,7 +4327,7 @@
       <c r="T10" s="10"/>
       <c r="U10" s="10"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>350</v>
       </c>
@@ -4343,7 +4346,7 @@
       <c r="T11" s="10"/>
       <c r="U11" s="10"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>400</v>
       </c>
@@ -4358,7 +4361,7 @@
       <c r="T12" s="10"/>
       <c r="U12" s="10"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>450</v>
       </c>
@@ -4373,7 +4376,7 @@
       <c r="T13" s="10"/>
       <c r="U13" s="10"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>500</v>
       </c>
@@ -4388,7 +4391,7 @@
       <c r="T14" s="10"/>
       <c r="U14" s="10"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>550</v>
       </c>
@@ -4403,7 +4406,7 @@
       <c r="T15" s="10"/>
       <c r="U15" s="10"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>600</v>
       </c>
@@ -4412,7 +4415,7 @@
       </c>
       <c r="C16" s="6"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>650</v>
       </c>
@@ -4421,7 +4424,7 @@
       </c>
       <c r="C17" s="6"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>700</v>
       </c>
@@ -4430,7 +4433,7 @@
       </c>
       <c r="C18" s="6"/>
     </row>
-    <row r="41" spans="1:21" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" ht="84.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="16" t="s">
         <v>19</v>
       </c>
@@ -4457,7 +4460,7 @@
       <c r="T41" s="17"/>
       <c r="U41" s="17"/>
     </row>
-    <row r="42" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="20" t="s">
         <v>14</v>
       </c>
@@ -4493,21 +4496,21 @@
       <selection activeCell="G36" sqref="G36:N36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="18" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="2"/>
+    <col min="3" max="3" width="9.1796875" style="2"/>
     <col min="4" max="5" width="18" style="2" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="2"/>
+    <col min="6" max="6" width="9.1796875" style="2"/>
     <col min="7" max="8" width="18" style="2" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="2"/>
+    <col min="9" max="9" width="9.1796875" style="2"/>
     <col min="10" max="11" width="18" style="2" customWidth="1"/>
-    <col min="12" max="12" width="11.28515625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="11.26953125" style="2" customWidth="1"/>
     <col min="13" max="14" width="18" style="2" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="2"/>
+    <col min="15" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>75</v>
       </c>
@@ -4529,7 +4532,7 @@
       </c>
       <c r="N1" s="16"/>
     </row>
-    <row r="3" spans="1:14" ht="18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -4561,7 +4564,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>-195.475113122171</v>
       </c>
@@ -4593,7 +4596,7 @@
         <v>13.2227855651655</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>-52.4886877828054</v>
       </c>
@@ -4625,7 +4628,7 @@
         <v>155.23173277661701</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>-22.624434389140202</v>
       </c>
@@ -4657,7 +4660,7 @@
         <v>164.140769460184</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>-3.6199095022624301</v>
       </c>
@@ -4689,7 +4692,7 @@
         <v>170.56606024455701</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>20.814479638009001</v>
       </c>
@@ -4721,7 +4724,7 @@
         <v>195.45600954369201</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>200.90497737556501</v>
       </c>
@@ -4753,7 +4756,7 @@
         <v>180.121682075753</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>400</v>
       </c>
@@ -4785,7 +4788,7 @@
         <v>196.49865791828199</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="G11" s="1">
         <v>22.743215031315199</v>
       </c>
@@ -4805,7 +4808,7 @@
         <v>267.01938562481303</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="G12" s="1">
         <v>39.774530271398703</v>
       </c>
@@ -4825,7 +4828,7 @@
         <v>267.12078735460699</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="G13" s="1">
         <v>59.986877423203097</v>
       </c>
@@ -4845,7 +4848,7 @@
         <v>269.22039964211098</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="G14" s="1">
         <v>70.293468535639704</v>
       </c>
@@ -4859,7 +4862,7 @@
         <v>276.25171488219502</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="M15" s="1">
         <v>60.0960334029227</v>
       </c>
@@ -4867,7 +4870,7 @@
         <v>300.66925141664098</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="M16" s="1">
         <v>59.741723829406503</v>
       </c>
@@ -4875,7 +4878,7 @@
         <v>248.06203399940301</v>
       </c>
     </row>
-    <row r="17" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="13:14" x14ac:dyDescent="0.35">
       <c r="M17" s="1">
         <v>-80.320906650760506</v>
       </c>
@@ -4883,7 +4886,7 @@
         <v>14.116313748881501</v>
       </c>
     </row>
-    <row r="18" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="13:14" x14ac:dyDescent="0.35">
       <c r="M18" s="1">
         <v>-70.226066209364703</v>
       </c>
@@ -4891,7 +4894,7 @@
         <v>14.662690128243399</v>
       </c>
     </row>
-    <row r="19" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="13:14" x14ac:dyDescent="0.35">
       <c r="M19" s="1">
         <v>-60.384730092454497</v>
       </c>
@@ -4899,7 +4902,7 @@
         <v>20.6668654935878</v>
       </c>
     </row>
-    <row r="20" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="13:14" x14ac:dyDescent="0.35">
       <c r="M20" s="1">
         <v>-50.168207575305701</v>
       </c>
@@ -4907,7 +4910,7 @@
         <v>170.593498359677</v>
       </c>
     </row>
-    <row r="21" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="13:14" x14ac:dyDescent="0.35">
       <c r="M21" s="1">
         <v>-40.341186996719301</v>
       </c>
@@ -4915,7 +4918,7 @@
         <v>182.55293766776001</v>
       </c>
     </row>
-    <row r="22" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="13:14" x14ac:dyDescent="0.35">
       <c r="M22" s="1">
         <v>-19.960035788845801</v>
       </c>
@@ -4923,7 +4926,7 @@
         <v>203.994035192365</v>
       </c>
     </row>
-    <row r="23" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="13:14" x14ac:dyDescent="0.35">
       <c r="M23" s="1">
         <v>-7.8735460781359706E-2</v>
       </c>
@@ -4931,7 +4934,7 @@
         <v>233.37309871756599</v>
       </c>
     </row>
-    <row r="24" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="13:14" x14ac:dyDescent="0.35">
       <c r="M24" s="1">
         <v>23.428571428571399</v>
       </c>
@@ -4939,7 +4942,7 @@
         <v>254.33343274679299</v>
       </c>
     </row>
-    <row r="25" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="13:14" x14ac:dyDescent="0.35">
       <c r="M25" s="1">
         <v>39.994631673128502</v>
       </c>
@@ -4947,7 +4950,7 @@
         <v>262.85237101103399</v>
       </c>
     </row>
-    <row r="26" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="13:14" x14ac:dyDescent="0.35">
       <c r="M26" s="1">
         <v>60.162839248434203</v>
       </c>
@@ -4955,7 +4958,7 @@
         <v>272.87801968386498</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" ht="79.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="16" t="s">
         <v>76</v>
       </c>
@@ -4997,26 +5000,26 @@
       <selection activeCell="M34" sqref="M34:N34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="2"/>
-    <col min="4" max="4" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" style="2"/>
+    <col min="4" max="4" width="8.26953125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="2"/>
-    <col min="7" max="7" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="2"/>
-    <col min="10" max="10" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" style="2"/>
+    <col min="7" max="7" width="8.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.1796875" style="2"/>
+    <col min="10" max="10" width="8.26953125" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.1796875" style="2" customWidth="1"/>
+    <col min="13" max="13" width="8.26953125" style="2" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="2"/>
+    <col min="15" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>47</v>
       </c>
@@ -5038,7 +5041,7 @@
       </c>
       <c r="N1" s="16"/>
     </row>
-    <row r="3" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>46</v>
       </c>
@@ -5070,7 +5073,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>10</v>
       </c>
@@ -5102,7 +5105,7 @@
         <v>95.557891687808393</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>30</v>
       </c>
@@ -5134,7 +5137,7 @@
         <v>88.682804290936701</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>100</v>
       </c>
@@ -5166,7 +5169,7 @@
         <v>81.200483429553103</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>300</v>
       </c>
@@ -5198,7 +5201,7 @@
         <v>74.529005773187606</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>1000</v>
       </c>
@@ -5230,7 +5233,7 @@
         <v>66.640813839669093</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>3000</v>
       </c>
@@ -5262,7 +5265,7 @@
         <v>60.172496454184</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>10000</v>
       </c>
@@ -5294,7 +5297,7 @@
         <v>52.487914261171703</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>30000</v>
       </c>
@@ -5326,7 +5329,7 @@
         <v>45.612377394674198</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>100000</v>
       </c>
@@ -5358,7 +5361,7 @@
         <v>37.927795201662001</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>300000</v>
       </c>
@@ -5390,7 +5393,7 @@
         <v>30.849547533909899</v>
       </c>
     </row>
-    <row r="32" spans="13:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="13:23" x14ac:dyDescent="0.35">
       <c r="M32" s="16"/>
       <c r="N32" s="16"/>
       <c r="O32" s="16"/>
@@ -5403,7 +5406,7 @@
       <c r="V32" s="16"/>
       <c r="W32" s="16"/>
     </row>
-    <row r="34" spans="1:23" ht="147" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" ht="147" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="16" t="s">
         <v>52</v>
       </c>
@@ -5456,25 +5459,25 @@
       <selection activeCell="P52" sqref="P52:T52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="13.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="2" customWidth="1"/>
-    <col min="4" max="5" width="13.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="2"/>
-    <col min="7" max="8" width="13.85546875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="2"/>
-    <col min="10" max="11" width="14.42578125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="2"/>
-    <col min="13" max="14" width="14.7109375" style="2" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" style="2"/>
-    <col min="16" max="17" width="15.28515625" style="2" customWidth="1"/>
-    <col min="18" max="18" width="9.140625" style="2"/>
-    <col min="19" max="20" width="15.28515625" style="2" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="2" width="13.453125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" style="2" customWidth="1"/>
+    <col min="4" max="5" width="13.453125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" style="2"/>
+    <col min="7" max="8" width="13.81640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="9.1796875" style="2"/>
+    <col min="10" max="11" width="14.453125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="9.1796875" style="2"/>
+    <col min="13" max="14" width="14.7265625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="9.1796875" style="2"/>
+    <col min="16" max="17" width="15.26953125" style="2" customWidth="1"/>
+    <col min="18" max="18" width="9.1796875" style="2"/>
+    <col min="19" max="20" width="15.26953125" style="2" customWidth="1"/>
+    <col min="21" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>41</v>
       </c>
@@ -5504,7 +5507,7 @@
       </c>
       <c r="T1" s="16"/>
     </row>
-    <row r="3" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>42</v>
       </c>
@@ -5548,7 +5551,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>4.8638199999999996</v>
       </c>
@@ -5592,7 +5595,7 @@
         <v>1.81249999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>9.9451300000000007</v>
       </c>
@@ -5636,7 +5639,7 @@
         <v>1.61029411764705</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>24.994789999999998</v>
       </c>
@@ -5680,7 +5683,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>48.371310000000001</v>
       </c>
@@ -5724,7 +5727,7 @@
         <v>1.4117647058823499</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>100.27548</v>
       </c>
@@ -5768,7 +5771,7 @@
         <v>1.41911764705882</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>252.01924</v>
       </c>
@@ -5812,7 +5815,7 @@
         <v>1.41911764705882</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>494.47662000000003</v>
       </c>
@@ -5856,7 +5859,7 @@
         <v>1.4117647058823499</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>50270.617209999997</v>
       </c>
@@ -5900,7 +5903,7 @@
         <v>1.40808823529411</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>98633.9179</v>
       </c>
@@ -5938,7 +5941,7 @@
         <v>1.2242647058823499</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>207303.64079999999</v>
       </c>
@@ -5976,7 +5979,7 @@
         <v>1.01838235294117</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>506872.17005999997</v>
       </c>
@@ -6008,7 +6011,7 @@
         <v>0.91911764705882304</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>1000000</v>
       </c>
@@ -6040,7 +6043,7 @@
         <v>0.91544117647058798</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="D16" s="2">
         <v>1008287.14299</v>
       </c>
@@ -6060,7 +6063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="16:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="16:20" x14ac:dyDescent="0.35">
       <c r="P17">
         <v>1608.5055696074701</v>
       </c>
@@ -6074,7 +6077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="16:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="16:20" x14ac:dyDescent="0.35">
       <c r="P18">
         <v>1254.92984463937</v>
       </c>
@@ -6088,7 +6091,7 @@
         <v>0.81617647058823495</v>
       </c>
     </row>
-    <row r="19" spans="16:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="16:20" x14ac:dyDescent="0.35">
       <c r="P19">
         <v>1352.9212213830299</v>
       </c>
@@ -6102,7 +6105,7 @@
         <v>0.81617647058823495</v>
       </c>
     </row>
-    <row r="20" spans="16:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="16:20" x14ac:dyDescent="0.35">
       <c r="P20">
         <v>1472.54042762412</v>
       </c>
@@ -6116,7 +6119,7 @@
         <v>0.8125</v>
       </c>
     </row>
-    <row r="21" spans="16:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="16:20" x14ac:dyDescent="0.35">
       <c r="P21">
         <v>1528.95166956412</v>
       </c>
@@ -6130,7 +6133,7 @@
         <v>0.81985294117647001</v>
       </c>
     </row>
-    <row r="22" spans="16:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="16:20" x14ac:dyDescent="0.35">
       <c r="P22">
         <v>1663.9047110839299</v>
       </c>
@@ -6144,7 +6147,7 @@
         <v>0.8125</v>
       </c>
     </row>
-    <row r="23" spans="16:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="16:20" x14ac:dyDescent="0.35">
       <c r="P23">
         <v>1551.94508748353</v>
       </c>
@@ -6158,7 +6161,7 @@
         <v>0.66176470588235303</v>
       </c>
     </row>
-    <row r="24" spans="16:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="16:20" x14ac:dyDescent="0.35">
       <c r="P24">
         <v>2156.4207065729001</v>
       </c>
@@ -6172,7 +6175,7 @@
         <v>0.60294117647058798</v>
       </c>
     </row>
-    <row r="25" spans="16:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="16:20" x14ac:dyDescent="0.35">
       <c r="P25">
         <v>2273.3309522936602</v>
       </c>
@@ -6186,7 +6189,7 @@
         <v>0.39705882352941102</v>
       </c>
     </row>
-    <row r="26" spans="16:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="16:20" x14ac:dyDescent="0.35">
       <c r="P26">
         <v>2450.8443254601498</v>
       </c>
@@ -6200,7 +6203,7 @@
         <v>0.51102941176470495</v>
       </c>
     </row>
-    <row r="27" spans="16:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="16:20" x14ac:dyDescent="0.35">
       <c r="P27">
         <v>3099.5348132387398</v>
       </c>
@@ -6214,7 +6217,7 @@
         <v>0.51102941176470495</v>
       </c>
     </row>
-    <row r="28" spans="16:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="16:20" x14ac:dyDescent="0.35">
       <c r="P28">
         <v>5296.0195526859297</v>
       </c>
@@ -6228,7 +6231,7 @@
         <v>0.51102941176470495</v>
       </c>
     </row>
-    <row r="29" spans="16:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="16:20" x14ac:dyDescent="0.35">
       <c r="P29">
         <v>5090.0575080803101</v>
       </c>
@@ -6236,7 +6239,7 @@
         <v>0.54411764705882304</v>
       </c>
     </row>
-    <row r="30" spans="16:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="16:20" x14ac:dyDescent="0.35">
       <c r="P30">
         <v>5324.6432593392001</v>
       </c>
@@ -6244,7 +6247,7 @@
         <v>0.49264705882352899</v>
       </c>
     </row>
-    <row r="31" spans="16:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="16:20" x14ac:dyDescent="0.35">
       <c r="P31">
         <v>7126.5797989979101</v>
       </c>
@@ -6252,7 +6255,7 @@
         <v>0.496323529411764</v>
       </c>
     </row>
-    <row r="32" spans="16:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="16:20" x14ac:dyDescent="0.35">
       <c r="P32">
         <v>8205.51119349898</v>
       </c>
@@ -6260,7 +6263,7 @@
         <v>0.496323529411764</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="P33">
         <v>12154.970287534299</v>
       </c>
@@ -6268,7 +6271,7 @@
         <v>0.44852941176470501</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="P34">
         <v>25018.3868587463</v>
       </c>
@@ -6276,7 +6279,7 @@
         <v>0.40073529411764702</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="16" t="s">
         <v>45</v>
       </c>
@@ -6295,7 +6298,7 @@
       <c r="M39" s="16"/>
       <c r="N39" s="16"/>
     </row>
-    <row r="52" spans="16:20" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="16:20" ht="93.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="P52" s="16" t="s">
         <v>60</v>
       </c>
@@ -6331,7 +6334,7 @@
       <selection activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6345,13 +6348,13 @@
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="26" width="12.5703125" style="10" customWidth="1"/>
-    <col min="27" max="16384" width="8.85546875" style="10"/>
+    <col min="1" max="26" width="12.54296875" style="10" customWidth="1"/>
+    <col min="27" max="16384" width="8.81640625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>6</v>
       </c>
@@ -6359,13 +6362,13 @@
       <c r="D1" s="17"/>
       <c r="E1" s="17"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" ht="46.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="1" customFormat="1" ht="45.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -6374,7 +6377,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="10">
         <v>295.59585492227899</v>
       </c>
@@ -6382,7 +6385,7 @@
         <v>8.1640711902113403E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="10">
         <v>322.79792746113901</v>
       </c>
@@ -6390,7 +6393,7 @@
         <v>8.0789766407119004E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="10">
         <v>373.31606217616502</v>
       </c>
@@ -6398,7 +6401,7 @@
         <v>7.7536151279199106E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="10">
         <v>472.79792746113901</v>
       </c>
@@ -6406,7 +6409,7 @@
         <v>7.5784204671857605E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="10">
         <v>573.05699481865202</v>
       </c>
@@ -6414,7 +6417,7 @@
         <v>7.0728587319243599E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="10">
         <v>673.31606217616502</v>
       </c>
@@ -6422,7 +6425,7 @@
         <v>6.4822024471635098E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="10">
         <v>772.79792746114003</v>
       </c>
@@ -6430,7 +6433,7 @@
         <v>5.8014460511679598E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="10">
         <v>873.05699481865202</v>
       </c>
@@ -6438,13 +6441,13 @@
         <v>5.0255839822024397E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="156" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" ht="156" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="16" t="s">
         <v>7</v>
       </c>
       <c r="B36" s="16"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="12" t="s">
         <v>5</v>
       </c>
@@ -6466,19 +6469,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{234A6B1F-5943-445E-8C13-06397E85A588}">
-  <dimension ref="A1:Y49"/>
+  <dimension ref="A1:Y65"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50:F65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="26" width="12.5703125" style="2" customWidth="1"/>
-    <col min="27" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="26" width="12.54296875" style="2" customWidth="1"/>
+    <col min="27" max="16384" width="8.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>6</v>
       </c>
@@ -6488,7 +6491,7 @@
       </c>
       <c r="E1" s="16"/>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -6496,13 +6499,13 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>296.10389610389598</v>
       </c>
@@ -6510,13 +6513,14 @@
         <v>448.39537869062798</v>
       </c>
       <c r="D4" s="2">
-        <v>20.54795</v>
+        <f>F51+273</f>
+        <v>293.54795000000001</v>
       </c>
       <c r="E4" s="2">
         <v>454.68159000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>322.72727272727201</v>
       </c>
@@ -6524,13 +6528,14 @@
         <v>461.48908857509599</v>
       </c>
       <c r="D5" s="2">
-        <v>53.424660000000003</v>
+        <f>F52+273</f>
+        <v>326.42466000000002</v>
       </c>
       <c r="E5" s="2">
         <v>467.34913999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>348.05194805194799</v>
       </c>
@@ -6538,13 +6543,14 @@
         <v>475.35301668806102</v>
       </c>
       <c r="D6" s="2">
-        <v>100</v>
+        <f>F53+273</f>
+        <v>373</v>
       </c>
       <c r="E6" s="2">
         <v>488.52064999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>373.376623376623</v>
       </c>
@@ -6552,13 +6558,14 @@
         <v>485.36585365853603</v>
       </c>
       <c r="D7" s="2">
-        <v>152.05479</v>
+        <f>F54+273</f>
+        <v>425.05479000000003</v>
       </c>
       <c r="E7" s="2">
         <v>509.65287000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>398.05194805194799</v>
       </c>
@@ -6566,13 +6573,14 @@
         <v>496.14890885750901</v>
       </c>
       <c r="D8" s="2">
-        <v>201.36985999999999</v>
+        <f>F55+273</f>
+        <v>474.36986000000002</v>
       </c>
       <c r="E8" s="2">
         <v>522.20258000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>423.376623376623</v>
       </c>
@@ -6580,13 +6588,14 @@
         <v>504.621309370988</v>
       </c>
       <c r="D9" s="2">
-        <v>250.68493000000001</v>
+        <f>F56+273</f>
+        <v>523.68493000000001</v>
       </c>
       <c r="E9" s="2">
         <v>543.35445000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>447.402597402597</v>
       </c>
@@ -6594,13 +6603,14 @@
         <v>513.86392811296503</v>
       </c>
       <c r="D10" s="2">
-        <v>300</v>
+        <f>F57+273</f>
+        <v>573</v>
       </c>
       <c r="E10" s="2">
         <v>551.60307999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>472.72727272727201</v>
       </c>
@@ -6608,13 +6618,14 @@
         <v>521.56611039794598</v>
       </c>
       <c r="D11" s="2">
-        <v>349.31506999999999</v>
+        <f>F58+273</f>
+        <v>622.31506999999999</v>
       </c>
       <c r="E11" s="2">
         <v>572.75495000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>498.05194805194799</v>
       </c>
@@ -6622,13 +6633,14 @@
         <v>530.03851091142405</v>
       </c>
       <c r="D12" s="2">
-        <v>398.63013999999998</v>
+        <f>F59+273</f>
+        <v>671.63013999999998</v>
       </c>
       <c r="E12" s="2">
         <v>585.30466000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>522.72727272727195</v>
       </c>
@@ -6636,13 +6648,14 @@
         <v>536.97047496790697</v>
       </c>
       <c r="D13" s="2">
-        <v>450.68493000000001</v>
+        <f>F60+273</f>
+        <v>723.68493000000001</v>
       </c>
       <c r="E13" s="2">
         <v>610.73796000000004</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>548.05194805194799</v>
       </c>
@@ -6650,13 +6663,14 @@
         <v>544.67265725288803</v>
       </c>
       <c r="D14" s="2">
-        <v>500</v>
+        <f>F61+273</f>
+        <v>773</v>
       </c>
       <c r="E14" s="2">
         <v>653.39520000000005</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>572.72727272727195</v>
       </c>
@@ -6664,13 +6678,14 @@
         <v>550.83440308087199</v>
       </c>
       <c r="D15" s="2">
-        <v>549.31506999999999</v>
+        <f>F62+273</f>
+        <v>822.31506999999999</v>
       </c>
       <c r="E15" s="2">
         <v>721.85888999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>598.05194805194799</v>
       </c>
@@ -6678,13 +6693,14 @@
         <v>556.99614890885698</v>
       </c>
       <c r="D16" s="2">
-        <v>598.63013999999998</v>
+        <f>F63+273</f>
+        <v>871.63013999999998</v>
       </c>
       <c r="E16" s="2">
         <v>803.22581000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>622.72727272727195</v>
       </c>
@@ -6692,13 +6708,14 @@
         <v>565.46854942233597</v>
       </c>
       <c r="D17" s="2">
-        <v>647.94520999999997</v>
+        <f>F64+273</f>
+        <v>920.94520999999997</v>
       </c>
       <c r="E17" s="2">
         <v>901.79701999999997</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>648.05194805194799</v>
       </c>
@@ -6706,13 +6723,14 @@
         <v>573.17073170731703</v>
       </c>
       <c r="D18" s="2">
-        <v>700</v>
+        <f>F65+273</f>
+        <v>973</v>
       </c>
       <c r="E18" s="2">
         <v>1026.1550500000001</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>673.376623376623</v>
       </c>
@@ -6720,7 +6738,7 @@
         <v>583.95378690629002</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>698.05194805194799</v>
       </c>
@@ -6728,7 +6746,7 @@
         <v>597.04749679075701</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>722.72727272727195</v>
       </c>
@@ -6736,7 +6754,7 @@
         <v>611.68164313221996</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>747.40259740259705</v>
       </c>
@@ -6744,7 +6762,7 @@
         <v>628.62644415917805</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>773.376623376623</v>
       </c>
@@ -6752,7 +6770,7 @@
         <v>655.58408215661098</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>797.40259740259705</v>
       </c>
@@ -6760,7 +6778,7 @@
         <v>687.16302952503202</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>822.72727272727195</v>
       </c>
@@ -6768,7 +6786,7 @@
         <v>721.05263157894694</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>847.40259740259705</v>
       </c>
@@ -6776,7 +6794,7 @@
         <v>764.18485237483901</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>872.72727272727195</v>
       </c>
@@ -6784,10 +6802,10 @@
         <v>801.155327342747</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.35">
       <c r="Y36" s="7"/>
     </row>
-    <row r="47" spans="1:25" ht="285" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:25" ht="285" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="16" t="s">
         <v>8</v>
       </c>
@@ -6797,9 +6815,89 @@
       </c>
       <c r="E47" s="16"/>
     </row>
-    <row r="49" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A49" s="7" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F50" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F51" s="2">
+        <v>20.54795</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F52" s="2">
+        <v>53.424660000000003</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F53" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F54" s="2">
+        <v>152.05479</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F55" s="2">
+        <v>201.36985999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F56" s="2">
+        <v>250.68493000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F57" s="2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F58" s="2">
+        <v>349.31506999999999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F59" s="2">
+        <v>398.63013999999998</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F60" s="2">
+        <v>450.68493000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F61" s="2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F62" s="2">
+        <v>549.31506999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F63" s="2">
+        <v>598.63013999999998</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F64" s="2">
+        <v>647.94520999999997</v>
+      </c>
+    </row>
+    <row r="65" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F65" s="2">
+        <v>700</v>
       </c>
     </row>
   </sheetData>
@@ -6819,19 +6917,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D45C8D-0E1D-4271-9C84-7C91BB3EB92B}">
-  <dimension ref="A1:V39"/>
+  <dimension ref="A1:V49"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5:D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="26" width="12.5703125" style="2" customWidth="1"/>
-    <col min="27" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="26" width="12.54296875" style="2" customWidth="1"/>
+    <col min="27" max="16384" width="8.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>6</v>
       </c>
@@ -6841,7 +6939,7 @@
       </c>
       <c r="E1" s="16"/>
     </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -6849,13 +6947,13 @@
         <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>295.83333333333297</v>
       </c>
@@ -6863,13 +6961,14 @@
         <v>28.330097087378601</v>
       </c>
       <c r="D4" s="2">
-        <v>20.54795</v>
+        <f>D37+273</f>
+        <v>293.54795000000001</v>
       </c>
       <c r="E4" s="2">
         <v>28.158940000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>322.61904761904702</v>
       </c>
@@ -6877,13 +6976,14 @@
         <v>28.932038834951399</v>
       </c>
       <c r="D5" s="2">
-        <v>50.684930000000001</v>
+        <f t="shared" ref="D5:D16" si="0">D38+273</f>
+        <v>323.68493000000001</v>
       </c>
       <c r="E5" s="2">
         <v>28.887419999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>372.61904761904702</v>
       </c>
@@ -6891,13 +6991,14 @@
         <v>29.194174757281498</v>
       </c>
       <c r="D6" s="2">
-        <v>102.73972999999999</v>
+        <f t="shared" si="0"/>
+        <v>375.73973000000001</v>
       </c>
       <c r="E6" s="2">
         <v>29.748339999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>473.21428571428498</v>
       </c>
@@ -6905,13 +7006,14 @@
         <v>30.6699029126213</v>
       </c>
       <c r="D7" s="2">
-        <v>152.05479</v>
+        <f t="shared" si="0"/>
+        <v>425.05479000000003</v>
       </c>
       <c r="E7" s="2">
         <v>30.27815</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>572.61904761904702</v>
       </c>
@@ -6919,13 +7021,14 @@
         <v>30.194174757281498</v>
       </c>
       <c r="D8" s="2">
-        <v>201.36985999999999</v>
+        <f t="shared" si="0"/>
+        <v>474.36986000000002</v>
       </c>
       <c r="E8" s="2">
         <v>30.344370000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>672.61904761904702</v>
       </c>
@@ -6933,13 +7036,14 @@
         <v>29.330097087378601</v>
       </c>
       <c r="D9" s="2">
-        <v>253.42465999999999</v>
+        <f t="shared" si="0"/>
+        <v>526.42466000000002</v>
       </c>
       <c r="E9" s="2">
         <v>30.211919999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>772.61904761904702</v>
       </c>
@@ -6947,13 +7051,14 @@
         <v>29.446601941747499</v>
       </c>
       <c r="D10" s="2">
-        <v>300</v>
+        <f t="shared" si="0"/>
+        <v>573</v>
       </c>
       <c r="E10" s="2">
         <v>29.947019999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>872.61904761904702</v>
       </c>
@@ -6961,53 +7066,59 @@
         <v>31.174757281553301</v>
       </c>
       <c r="D11" s="2">
-        <v>352.05479000000003</v>
+        <f t="shared" si="0"/>
+        <v>625.05479000000003</v>
       </c>
       <c r="E11" s="2">
         <v>29.682120000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D12" s="2">
-        <v>401.36986000000002</v>
+        <f t="shared" si="0"/>
+        <v>674.36986000000002</v>
       </c>
       <c r="E12" s="2">
         <v>29.483440000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D13" s="2">
-        <v>450.68493000000001</v>
+        <f t="shared" si="0"/>
+        <v>723.68493000000001</v>
       </c>
       <c r="E13" s="2">
         <v>29.350989999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D14" s="2">
-        <v>502.73973000000001</v>
+        <f t="shared" si="0"/>
+        <v>775.73973000000001</v>
       </c>
       <c r="E14" s="2">
         <v>29.61589</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D15" s="2">
-        <v>552.05479000000003</v>
+        <f t="shared" si="0"/>
+        <v>825.05479000000003</v>
       </c>
       <c r="E15" s="2">
         <v>30.079470000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D16" s="2">
-        <v>601.36986000000002</v>
+        <f t="shared" si="0"/>
+        <v>874.36986000000002</v>
       </c>
       <c r="E16" s="2">
         <v>31.13907</v>
       </c>
     </row>
-    <row r="33" spans="1:22" ht="208.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" ht="208.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="16" t="s">
         <v>9</v>
       </c>
@@ -7017,13 +7128,81 @@
       </c>
       <c r="E33" s="16"/>
     </row>
-    <row r="35" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="D36" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="D37" s="2">
+        <v>20.54795</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="D38" s="2">
+        <v>50.684930000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="D39" s="2">
+        <v>102.73972999999999</v>
+      </c>
       <c r="V39" s="7"/>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="D40" s="2">
+        <v>152.05479</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="D41" s="2">
+        <v>201.36985999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="D42" s="2">
+        <v>253.42465999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="D43" s="2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="D44" s="2">
+        <v>352.05479000000003</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="D45" s="2">
+        <v>401.36986000000002</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="D46" s="2">
+        <v>450.68493000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="D47" s="2">
+        <v>502.73973000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="D48" s="2">
+        <v>552.05479000000003</v>
+      </c>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D49" s="2">
+        <v>601.36986000000002</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -7044,21 +7223,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B14F85A-DEBE-455F-A23B-C51456BB79FE}">
   <dimension ref="A1:V55"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="A53" sqref="A53:B53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" style="10" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" style="10"/>
-    <col min="4" max="4" width="16.42578125" style="10" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" style="10" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="10"/>
+    <col min="1" max="1" width="15.453125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="21.81640625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="8.81640625" style="10"/>
+    <col min="4" max="4" width="16.453125" style="10" customWidth="1"/>
+    <col min="5" max="5" width="20.453125" style="10" customWidth="1"/>
+    <col min="6" max="16384" width="8.81640625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>6</v>
       </c>
@@ -7066,13 +7245,13 @@
       <c r="D1" s="17"/>
       <c r="E1" s="17"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="33" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -7082,7 +7261,7 @@
       <c r="D3" s="1"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="10">
         <v>303.31797235022998</v>
       </c>
@@ -7090,7 +7269,7 @@
         <v>51.077844311377198</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="10">
         <v>327.64976958525301</v>
       </c>
@@ -7098,7 +7277,7 @@
         <v>54.550898203592801</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="10">
         <v>344.23963133640501</v>
       </c>
@@ -7106,7 +7285,7 @@
         <v>56.467065868263397</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="10">
         <v>365.806451612903</v>
       </c>
@@ -7114,7 +7293,7 @@
         <v>59.101796407185603</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="10">
         <v>396.22119815668202</v>
       </c>
@@ -7122,7 +7301,7 @@
         <v>62.814371257485</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="10">
         <v>423.31797235022998</v>
       </c>
@@ -7130,7 +7309,7 @@
         <v>66.407185628742496</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="10">
         <v>450.41474654377799</v>
       </c>
@@ -7138,7 +7317,7 @@
         <v>69.281437125748496</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="10">
         <v>467.00460829492999</v>
       </c>
@@ -7146,7 +7325,7 @@
         <v>71.437125748502893</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="10">
         <v>497.41935483870901</v>
       </c>
@@ -7154,7 +7333,7 @@
         <v>75.508982035928099</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="10">
         <v>523.41013824884703</v>
       </c>
@@ -7162,7 +7341,7 @@
         <v>77.425149700598794</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="10">
         <v>545.52995391704997</v>
       </c>
@@ -7170,7 +7349,7 @@
         <v>81.137724550898199</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="10">
         <v>577.05069124423903</v>
       </c>
@@ -7178,7 +7357,7 @@
         <v>84.730538922155603</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="10">
         <v>601.935483870967</v>
       </c>
@@ -7186,7 +7365,7 @@
         <v>87.245508982035901</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="10">
         <v>657.78801843317899</v>
       </c>
@@ -7194,7 +7373,7 @@
         <v>93.473053892215503</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="10">
         <v>682.11981566820202</v>
       </c>
@@ -7202,7 +7381,7 @@
         <v>96.227544910179603</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="10">
         <v>708.11059907834101</v>
       </c>
@@ -7210,7 +7389,7 @@
         <v>99.580838323353206</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="10">
         <v>734.65437788018403</v>
       </c>
@@ -7218,7 +7397,7 @@
         <v>102.57485029940101</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="10">
         <v>763.41013824884703</v>
       </c>
@@ -7226,7 +7405,7 @@
         <v>105.808383233532</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="10">
         <v>783.87096774193503</v>
       </c>
@@ -7234,7 +7413,7 @@
         <v>107.96407185628701</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="10">
         <v>817.05069124423903</v>
       </c>
@@ -7242,7 +7421,7 @@
         <v>111.19760479041901</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="10">
         <v>850.23041474654303</v>
       </c>
@@ -7250,7 +7429,7 @@
         <v>114.19161676646701</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="10">
         <v>883.963133640553</v>
       </c>
@@ -7258,7 +7437,7 @@
         <v>117.425149700598</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="10">
         <v>924.88479262672797</v>
       </c>
@@ -7266,16 +7445,16 @@
         <v>121.377245508982</v>
       </c>
     </row>
-    <row r="37" spans="22:22" x14ac:dyDescent="0.25">
+    <row r="37" spans="22:22" x14ac:dyDescent="0.35">
       <c r="V37" s="12"/>
     </row>
-    <row r="53" spans="1:2" ht="210" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" ht="210" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="16" t="s">
         <v>10</v>
       </c>
       <c r="B53" s="16"/>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="12" t="s">
         <v>5</v>
       </c>
@@ -7302,18 +7481,18 @@
       <selection activeCell="A39" sqref="A39:B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="12.5703125" style="2"/>
+    <col min="1" max="16384" width="12.54296875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="16"/>
     </row>
-    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -7321,7 +7500,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>100</v>
       </c>
@@ -7329,7 +7508,7 @@
         <v>10.6898734177215</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>200</v>
       </c>
@@ -7337,7 +7516,7 @@
         <v>11.0443037974683</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>300</v>
       </c>
@@ -7345,7 +7524,7 @@
         <v>11.386075949366999</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>400</v>
       </c>
@@ -7353,7 +7532,7 @@
         <v>11.6962025316455</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>500</v>
       </c>
@@ -7361,7 +7540,7 @@
         <v>11.987341772151799</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>600</v>
       </c>
@@ -7369,7 +7548,7 @@
         <v>12.246835443037901</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>700</v>
       </c>
@@ -7377,13 +7556,13 @@
         <v>12.487341772151799</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="187.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" ht="187.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="16" t="s">
         <v>13</v>
       </c>
       <c r="B39" s="16"/>
     </row>
-    <row r="40" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" s="7" t="s">
         <v>14</v>
       </c>
@@ -7409,12 +7588,12 @@
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="12.5703125" style="2"/>
+    <col min="1" max="16384" width="12.54296875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>21</v>
       </c>
@@ -7429,7 +7608,7 @@
       <c r="H1" s="16"/>
       <c r="I1" s="11"/>
     </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
@@ -7449,7 +7628,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="9">
         <v>473.100871731008</v>
       </c>
@@ -7469,7 +7648,7 @@
         <v>8.3535353535353393E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="9">
         <v>573.22540473225399</v>
       </c>
@@ -7489,7 +7668,7 @@
         <v>0.10090909090909</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="9">
         <v>672.97633872976303</v>
       </c>
@@ -7509,7 +7688,7 @@
         <v>0.12030303030303</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="9">
         <v>772.72727272727195</v>
       </c>
@@ -7529,7 +7708,7 @@
         <v>0.14070707070707</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="9">
         <v>872.851805728518</v>
       </c>
@@ -7549,11 +7728,11 @@
         <v>0.16292929292929201</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="9"/>
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
@@ -7568,7 +7747,7 @@
       <c r="L32" s="9"/>
       <c r="M32" s="9"/>
     </row>
-    <row r="33" spans="1:14" ht="153" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="153" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="18" t="s">
         <v>24</v>
       </c>
@@ -7590,7 +7769,7 @@
       <c r="M33" s="18"/>
       <c r="N33" s="18"/>
     </row>
-    <row r="34" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A34" s="9" t="s">
         <v>20</v>
       </c>
@@ -7620,19 +7799,19 @@
       <selection activeCell="A4" sqref="A4:A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" style="5" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="12.81640625" style="5" customWidth="1"/>
+    <col min="2" max="16384" width="9.1796875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
         <v>67</v>
       </c>
       <c r="B1" s="19"/>
     </row>
-    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -7640,7 +7819,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>17.541148288385699</v>
       </c>
@@ -7648,7 +7827,7 @@
         <v>33.767998351492601</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>147.82474306467799</v>
       </c>
@@ -7656,7 +7835,7 @@
         <v>32.228318264945997</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>297.73587821652097</v>
       </c>
@@ -7664,7 +7843,7 @@
         <v>36.684439636298002</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>447.708832393168</v>
       </c>
@@ -7672,7 +7851,7 @@
         <v>40.214563531926899</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>498.24588517116098</v>
       </c>
@@ -7680,7 +7859,7 @@
         <v>33.211627128248601</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>548.53566184993394</v>
       </c>
@@ -7688,7 +7867,7 @@
         <v>29.912680627463001</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>599.16544316513398</v>
       </c>
@@ -7696,7 +7875,7 @@
         <v>21.520748010200101</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>648.18792983540595</v>
       </c>
@@ -7704,7 +7883,7 @@
         <v>20.538083095072398</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>698.81771115060599</v>
       </c>
@@ -7712,7 +7891,7 @@
         <v>12.1461504778094</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="179.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="179.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="16" t="s">
         <v>68</v>
       </c>
@@ -7736,23 +7915,23 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="10.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1796875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="10.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1796875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="10.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>87</v>
       </c>
@@ -7770,7 +7949,7 @@
       </c>
       <c r="K1" s="16"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -7783,7 +7962,7 @@
       <c r="J2" s="11"/>
       <c r="K2" s="11"/>
     </row>
-    <row r="3" spans="1:11" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="33.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>84</v>
       </c>
@@ -7809,7 +7988,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>20</v>
       </c>
@@ -7835,7 +8014,7 @@
         <v>420.225490196078</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>650</v>
       </c>
@@ -7861,7 +8040,7 @@
         <v>300.225490196078</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>700</v>
       </c>
@@ -7887,7 +8066,7 @@
         <v>255.04901960784301</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>725</v>
       </c>
@@ -7913,7 +8092,7 @@
         <v>210.225490196078</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>775</v>
       </c>
@@ -7939,7 +8118,7 @@
         <v>199.99019607843101</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>825</v>
       </c>
@@ -7965,7 +8144,7 @@
         <v>202.81372549019599</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>850</v>
       </c>
@@ -7991,7 +8170,7 @@
         <v>394.81372549019602</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>950</v>
       </c>
@@ -8017,7 +8196,7 @@
         <v>410.34313725490199</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>1000</v>
       </c>
@@ -8031,7 +8210,7 @@
         <v>419.85294117646998</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>1050</v>
       </c>
@@ -8045,7 +8224,7 @@
         <v>417.15686274509801</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>1100</v>
       </c>
@@ -8059,7 +8238,7 @@
         <v>414.70588235294099</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>1150</v>
       </c>
@@ -8073,7 +8252,7 @@
         <v>394.85294117646998</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="53.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="16" t="s">
         <v>86</v>
       </c>

</xml_diff>

<commit_message>
various updates to V1.0 and applied to Eurofer
</commit_message>
<xml_diff>
--- a/Jupyter/Eurofer/Eurofer_data.xlsx
+++ b/Jupyter/Eurofer/Eurofer_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Research\Repos\DatabaseCodes\Jupyter\Eurofer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE03CF13-0199-4EF8-8DB8-7B60A609EBEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5852CB07-8AC2-4253-A80D-3CE00E7CA3CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="852" activeTab="3" xr2:uid="{D289EE42-B074-4616-9B9B-4CE9F1662138}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="852" activeTab="10" xr2:uid="{D289EE42-B074-4616-9B9B-4CE9F1662138}"/>
   </bookViews>
   <sheets>
     <sheet name="Eurofer_density" sheetId="15" r:id="rId1"/>
@@ -30,6 +30,7 @@
     <sheet name="Eurofer_chemical" sheetId="13" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1995,14 +1996,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>38101</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>157529</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>138479</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>114301</xdr:rowOff>
     </xdr:to>
@@ -2039,13 +2040,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>333900</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>124002</xdr:rowOff>
@@ -2083,16 +2084,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>39</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>52</xdr:col>
-      <xdr:colOff>315052</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>10083</xdr:rowOff>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>467452</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>1299133</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2115,8 +2116,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="21021675" y="3800475"/>
-          <a:ext cx="5210902" cy="4001058"/>
+          <a:off x="22958425" y="5737225"/>
+          <a:ext cx="5442677" cy="3867708"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2127,16 +2128,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>263525</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>73025</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>315060</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>19604</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>188060</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>1334054</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2159,8 +2160,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14525625" y="3838575"/>
-          <a:ext cx="5268060" cy="3972479"/>
+          <a:off x="15039975" y="5800725"/>
+          <a:ext cx="5518885" cy="3839129"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2580,1035 +2581,1625 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{689ABF1C-EFBF-442E-A0BE-50F31494446C}">
-  <dimension ref="A1:BJ40"/>
+  <dimension ref="A1:EQ40"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="12.54296875" style="2"/>
-    <col min="3" max="3" width="12.54296875" style="2" customWidth="1"/>
-    <col min="4" max="9" width="12.54296875" style="2"/>
-    <col min="10" max="14" width="12.81640625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="12.54296875" style="2"/>
-    <col min="16" max="16" width="5.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="2.453125" style="2" customWidth="1"/>
-    <col min="19" max="19" width="5.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="3.54296875" style="2" customWidth="1"/>
-    <col min="22" max="22" width="5.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="2.81640625" style="2" customWidth="1"/>
-    <col min="25" max="25" width="5.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="3.54296875" style="2" customWidth="1"/>
-    <col min="28" max="28" width="5.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="3" style="2" customWidth="1"/>
-    <col min="31" max="31" width="5.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="3.54296875" style="2" customWidth="1"/>
-    <col min="34" max="34" width="5.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="3.453125" style="2" customWidth="1"/>
-    <col min="37" max="37" width="5.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="3.54296875" style="2" customWidth="1"/>
-    <col min="40" max="40" width="5.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="3.26953125" style="2" customWidth="1"/>
-    <col min="43" max="43" width="5.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="3.54296875" style="2" customWidth="1"/>
-    <col min="46" max="46" width="5.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="2.1796875" style="2" customWidth="1"/>
-    <col min="49" max="49" width="5.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="3.54296875" style="2" customWidth="1"/>
-    <col min="52" max="52" width="5.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="5" style="2" customWidth="1"/>
-    <col min="55" max="55" width="5.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="3.54296875" style="2" customWidth="1"/>
-    <col min="58" max="58" width="5.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="3.1796875" style="2" customWidth="1"/>
-    <col min="61" max="61" width="5.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="63" max="16384" width="12.54296875" style="2"/>
+    <col min="1" max="6" width="12.54296875" style="2"/>
+    <col min="7" max="10" width="12.81640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="5.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.453125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="5.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="3.54296875" style="2" customWidth="1"/>
+    <col min="17" max="17" width="5.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="2.81640625" style="2" customWidth="1"/>
+    <col min="20" max="20" width="5.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="3.54296875" style="2" customWidth="1"/>
+    <col min="23" max="23" width="5.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="3" style="2" customWidth="1"/>
+    <col min="26" max="26" width="5.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="3.54296875" style="2" customWidth="1"/>
+    <col min="29" max="29" width="5.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="3.453125" style="2" customWidth="1"/>
+    <col min="32" max="32" width="5.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="3.54296875" style="2" customWidth="1"/>
+    <col min="35" max="35" width="5.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="3.26953125" style="2" customWidth="1"/>
+    <col min="38" max="38" width="5.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="3.54296875" style="2" customWidth="1"/>
+    <col min="41" max="41" width="5.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="2.1796875" style="2" customWidth="1"/>
+    <col min="44" max="44" width="5.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="3.54296875" style="2" customWidth="1"/>
+    <col min="47" max="47" width="5.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="5" style="2" customWidth="1"/>
+    <col min="50" max="50" width="5.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="3.54296875" style="2" customWidth="1"/>
+    <col min="53" max="53" width="5.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="3.1796875" style="2" customWidth="1"/>
+    <col min="56" max="56" width="5.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="58" max="16384" width="12.54296875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:147" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="16"/>
-      <c r="D1" s="16" t="s">
+      <c r="C1" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="16"/>
       <c r="G1" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="L1" s="16"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="O1" s="16"/>
+      <c r="Q1" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="R1" s="16"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="U1" s="16"/>
+      <c r="W1" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA1" s="16"/>
+      <c r="AC1" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD1" s="16"/>
+      <c r="AE1" s="11"/>
+      <c r="AF1" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="AG1" s="16"/>
+      <c r="AI1" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="AJ1" s="16"/>
+      <c r="AK1" s="11"/>
+      <c r="AL1" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="AM1" s="16"/>
+      <c r="AO1" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="AP1" s="16"/>
+      <c r="AQ1" s="11"/>
+      <c r="AR1" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="AS1" s="16"/>
+      <c r="AU1" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="AV1" s="16"/>
+      <c r="AW1" s="11"/>
+      <c r="AX1" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="AY1" s="16"/>
+      <c r="BA1" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="BB1" s="16"/>
+      <c r="BC1" s="11"/>
+      <c r="BD1" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="BE1" s="16"/>
+    </row>
+    <row r="2" spans="1:147" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <f>A2+1</f>
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <f t="shared" ref="C2:BN2" si="0">B2+1</f>
+        <v>2</v>
+      </c>
+      <c r="D2" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E2" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F2" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G2" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="H2" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="I2" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="J2" s="2">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="K2" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="L2" s="2">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="M2" s="2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="N2" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="O2" s="2">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="P2" s="2">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="Q2" s="2">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="R2" s="2">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="S2" s="2">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="T2" s="2">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="U2" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="V2" s="2">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="W2" s="2">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="X2" s="2">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="Y2" s="2">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="Z2" s="2">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="AA2" s="2">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="AB2" s="2">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="AC2" s="2">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="AD2" s="2">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="AE2" s="2">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="AF2" s="2">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="AG2" s="2">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="AH2" s="2">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="AI2" s="2">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="AJ2" s="2">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="AK2" s="2">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="AL2" s="2">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="AM2" s="2">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="AN2" s="2">
+        <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="H1" s="16"/>
-      <c r="J1" s="16" t="s">
+      <c r="AO2" s="2">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="AP2" s="2">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="AQ2" s="2">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="AR2" s="2">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="AS2" s="2">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="AT2" s="2">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="AU2" s="2">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="AV2" s="2">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="AW2" s="2">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="AX2" s="2">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="AY2" s="2">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="AZ2" s="2">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="BA2" s="2">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="BB2" s="2">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="BC2" s="2">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="BD2" s="2">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="BE2" s="2">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="BF2" s="2">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="BG2" s="2">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="BH2" s="2">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="BI2" s="2">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="BJ2" s="2">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="BK2" s="2">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="BL2" s="2">
+        <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="K1" s="16"/>
-      <c r="M1" s="16" t="s">
+      <c r="BM2" s="2">
+        <f t="shared" si="0"/>
         <v>64</v>
       </c>
-      <c r="N1" s="16"/>
-      <c r="P1" s="16" t="s">
+      <c r="BN2" s="2">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="BO2" s="2">
+        <f t="shared" ref="BO2:DZ2" si="1">BN2+1</f>
+        <v>66</v>
+      </c>
+      <c r="BP2" s="2">
+        <f t="shared" si="1"/>
+        <v>67</v>
+      </c>
+      <c r="BQ2" s="2">
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+      <c r="BR2" s="2">
+        <f t="shared" si="1"/>
+        <v>69</v>
+      </c>
+      <c r="BS2" s="2">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="BT2" s="2">
+        <f t="shared" si="1"/>
+        <v>71</v>
+      </c>
+      <c r="BU2" s="2">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="BV2" s="2">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
+      <c r="BW2" s="2">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="BX2" s="2">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="BY2" s="2">
+        <f t="shared" si="1"/>
+        <v>76</v>
+      </c>
+      <c r="BZ2" s="2">
+        <f t="shared" si="1"/>
+        <v>77</v>
+      </c>
+      <c r="CA2" s="2">
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
+      <c r="CB2" s="2">
+        <f t="shared" si="1"/>
+        <v>79</v>
+      </c>
+      <c r="CC2" s="2">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="CD2" s="2">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
+      <c r="CE2" s="2">
+        <f t="shared" si="1"/>
+        <v>82</v>
+      </c>
+      <c r="CF2" s="2">
+        <f t="shared" si="1"/>
+        <v>83</v>
+      </c>
+      <c r="CG2" s="2">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+      <c r="CH2" s="2">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+      <c r="CI2" s="2">
+        <f t="shared" si="1"/>
+        <v>86</v>
+      </c>
+      <c r="CJ2" s="2">
+        <f t="shared" si="1"/>
+        <v>87</v>
+      </c>
+      <c r="CK2" s="2">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+      <c r="CL2" s="2">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+      <c r="CM2" s="2">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="CN2" s="2">
+        <f t="shared" si="1"/>
+        <v>91</v>
+      </c>
+      <c r="CO2" s="2">
+        <f t="shared" si="1"/>
         <v>92</v>
       </c>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="T1" s="16"/>
-      <c r="V1" s="16" t="s">
+      <c r="CP2" s="2">
+        <f t="shared" si="1"/>
         <v>93</v>
       </c>
-      <c r="W1" s="16"/>
-      <c r="X1" s="11"/>
-      <c r="Y1" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="Z1" s="16"/>
-      <c r="AB1" s="16" t="s">
+      <c r="CQ2" s="2">
+        <f t="shared" si="1"/>
         <v>94</v>
       </c>
-      <c r="AC1" s="16"/>
-      <c r="AD1" s="11"/>
-      <c r="AE1" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="AF1" s="16"/>
-      <c r="AH1" s="16" t="s">
+      <c r="CR2" s="2">
+        <f t="shared" si="1"/>
         <v>95</v>
       </c>
-      <c r="AI1" s="16"/>
-      <c r="AJ1" s="11"/>
-      <c r="AK1" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="AL1" s="16"/>
-      <c r="AN1" s="16" t="s">
+      <c r="CS2" s="2">
+        <f t="shared" si="1"/>
         <v>96</v>
       </c>
-      <c r="AO1" s="16"/>
-      <c r="AP1" s="11"/>
-      <c r="AQ1" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="AR1" s="16"/>
-      <c r="AT1" s="16" t="s">
+      <c r="CT2" s="2">
+        <f t="shared" si="1"/>
         <v>97</v>
       </c>
-      <c r="AU1" s="16"/>
-      <c r="AV1" s="11"/>
-      <c r="AW1" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="AX1" s="16"/>
-      <c r="AZ1" s="16" t="s">
+      <c r="CU2" s="2">
+        <f t="shared" si="1"/>
         <v>98</v>
       </c>
-      <c r="BA1" s="16"/>
-      <c r="BB1" s="11"/>
-      <c r="BC1" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="BD1" s="16"/>
-      <c r="BF1" s="16" t="s">
+      <c r="CV2" s="2">
+        <f t="shared" si="1"/>
         <v>99</v>
       </c>
-      <c r="BG1" s="16"/>
-      <c r="BH1" s="11"/>
-      <c r="BI1" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="BJ1" s="16"/>
-    </row>
-    <row r="2" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:62" ht="58" x14ac:dyDescent="0.35">
+      <c r="CW2" s="2">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="CX2" s="2">
+        <f t="shared" si="1"/>
+        <v>101</v>
+      </c>
+      <c r="CY2" s="2">
+        <f t="shared" si="1"/>
+        <v>102</v>
+      </c>
+      <c r="CZ2" s="2">
+        <f t="shared" si="1"/>
+        <v>103</v>
+      </c>
+      <c r="DA2" s="2">
+        <f t="shared" si="1"/>
+        <v>104</v>
+      </c>
+      <c r="DB2" s="2">
+        <f t="shared" si="1"/>
+        <v>105</v>
+      </c>
+      <c r="DC2" s="2">
+        <f t="shared" si="1"/>
+        <v>106</v>
+      </c>
+      <c r="DD2" s="2">
+        <f t="shared" si="1"/>
+        <v>107</v>
+      </c>
+      <c r="DE2" s="2">
+        <f t="shared" si="1"/>
+        <v>108</v>
+      </c>
+      <c r="DF2" s="2">
+        <f t="shared" si="1"/>
+        <v>109</v>
+      </c>
+      <c r="DG2" s="2">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+      <c r="DH2" s="2">
+        <f t="shared" si="1"/>
+        <v>111</v>
+      </c>
+      <c r="DI2" s="2">
+        <f t="shared" si="1"/>
+        <v>112</v>
+      </c>
+      <c r="DJ2" s="2">
+        <f t="shared" si="1"/>
+        <v>113</v>
+      </c>
+      <c r="DK2" s="2">
+        <f t="shared" si="1"/>
+        <v>114</v>
+      </c>
+      <c r="DL2" s="2">
+        <f t="shared" si="1"/>
+        <v>115</v>
+      </c>
+      <c r="DM2" s="2">
+        <f t="shared" si="1"/>
+        <v>116</v>
+      </c>
+      <c r="DN2" s="2">
+        <f t="shared" si="1"/>
+        <v>117</v>
+      </c>
+      <c r="DO2" s="2">
+        <f t="shared" si="1"/>
+        <v>118</v>
+      </c>
+      <c r="DP2" s="2">
+        <f t="shared" si="1"/>
+        <v>119</v>
+      </c>
+      <c r="DQ2" s="2">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+      <c r="DR2" s="2">
+        <f t="shared" si="1"/>
+        <v>121</v>
+      </c>
+      <c r="DS2" s="2">
+        <f t="shared" si="1"/>
+        <v>122</v>
+      </c>
+      <c r="DT2" s="2">
+        <f t="shared" si="1"/>
+        <v>123</v>
+      </c>
+      <c r="DU2" s="2">
+        <f t="shared" si="1"/>
+        <v>124</v>
+      </c>
+      <c r="DV2" s="2">
+        <f t="shared" si="1"/>
+        <v>125</v>
+      </c>
+      <c r="DW2" s="2">
+        <f t="shared" si="1"/>
+        <v>126</v>
+      </c>
+      <c r="DX2" s="2">
+        <f t="shared" si="1"/>
+        <v>127</v>
+      </c>
+      <c r="DY2" s="2">
+        <f t="shared" si="1"/>
+        <v>128</v>
+      </c>
+      <c r="DZ2" s="2">
+        <f t="shared" si="1"/>
+        <v>129</v>
+      </c>
+      <c r="EA2" s="2">
+        <f t="shared" ref="EA2:EQ2" si="2">DZ2+1</f>
+        <v>130</v>
+      </c>
+      <c r="EB2" s="2">
+        <f t="shared" si="2"/>
+        <v>131</v>
+      </c>
+      <c r="EC2" s="2">
+        <f t="shared" si="2"/>
+        <v>132</v>
+      </c>
+      <c r="ED2" s="2">
+        <f t="shared" si="2"/>
+        <v>133</v>
+      </c>
+      <c r="EE2" s="2">
+        <f t="shared" si="2"/>
+        <v>134</v>
+      </c>
+      <c r="EF2" s="2">
+        <f t="shared" si="2"/>
+        <v>135</v>
+      </c>
+      <c r="EG2" s="2">
+        <f t="shared" si="2"/>
+        <v>136</v>
+      </c>
+      <c r="EH2" s="2">
+        <f t="shared" si="2"/>
+        <v>137</v>
+      </c>
+      <c r="EI2" s="2">
+        <f t="shared" si="2"/>
+        <v>138</v>
+      </c>
+      <c r="EJ2" s="2">
+        <f t="shared" si="2"/>
+        <v>139</v>
+      </c>
+      <c r="EK2" s="2">
+        <f t="shared" si="2"/>
+        <v>140</v>
+      </c>
+      <c r="EL2" s="2">
+        <f t="shared" si="2"/>
+        <v>141</v>
+      </c>
+      <c r="EM2" s="2">
+        <f t="shared" si="2"/>
+        <v>142</v>
+      </c>
+      <c r="EN2" s="2">
+        <f t="shared" si="2"/>
+        <v>143</v>
+      </c>
+      <c r="EO2" s="2">
+        <f t="shared" si="2"/>
+        <v>144</v>
+      </c>
+      <c r="EP2" s="2">
+        <f t="shared" si="2"/>
+        <v>145</v>
+      </c>
+      <c r="EQ2" s="2">
+        <f t="shared" si="2"/>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:147" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="D3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>16</v>
+      <c r="F3" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="N3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="P3" s="2" t="s">
+      <c r="O3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="T3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="U3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="X3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="Z3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="T3" s="2" t="s">
+      <c r="AA3" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="V3" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="W3" s="2" t="s">
+      <c r="AC3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Y3" s="2" t="s">
+      <c r="AF3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Z3" s="2" t="s">
+      <c r="AG3" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="AB3" s="2" t="s">
+      <c r="AI3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="AC3" s="2" t="s">
+      <c r="AJ3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="AE3" s="2" t="s">
+      <c r="AL3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="AF3" s="2" t="s">
+      <c r="AM3" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="AH3" s="2" t="s">
+      <c r="AO3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="AI3" s="2" t="s">
+      <c r="AP3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="AK3" s="2" t="s">
+      <c r="AR3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="AL3" s="2" t="s">
+      <c r="AS3" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="AN3" s="2" t="s">
+      <c r="AU3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="AO3" s="2" t="s">
+      <c r="AV3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="AQ3" s="2" t="s">
+      <c r="AX3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="AR3" s="2" t="s">
+      <c r="AY3" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="AT3" s="2" t="s">
+      <c r="BA3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="AU3" s="2" t="s">
+      <c r="BB3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="AW3" s="2" t="s">
+      <c r="BD3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="AX3" s="2" t="s">
+      <c r="BE3" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="AZ3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="BA3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="BC3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="BD3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="BF3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="BG3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="BI3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="BJ3" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:62" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:147" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>20</v>
       </c>
       <c r="B4" s="8">
         <v>547.85809906291797</v>
       </c>
+      <c r="C4" s="2">
+        <v>20</v>
+      </c>
       <c r="D4" s="2">
+        <v>511.72883999999999</v>
+      </c>
+      <c r="E4" s="2">
         <v>20</v>
       </c>
-      <c r="E4" s="2">
-        <v>511.72883999999999</v>
-      </c>
-      <c r="G4" s="2">
-        <v>20</v>
+      <c r="F4" s="2">
+        <v>634.60653000000002</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="H4" s="2">
-        <v>634.60653000000002</v>
-      </c>
-      <c r="J4" s="2" t="s">
+        <v>886</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="K4" s="2">
-        <v>886</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="N4" s="2">
+      <c r="J4" s="2">
         <v>1066</v>
       </c>
-      <c r="P4" s="15">
+      <c r="K4" s="15">
         <v>18.947368421052602</v>
       </c>
+      <c r="L4" s="15">
+        <v>570.96774193548299</v>
+      </c>
+      <c r="M4" s="15"/>
+      <c r="N4" s="14">
+        <v>15</v>
+      </c>
+      <c r="O4" s="14">
+        <v>675.86206896551698</v>
+      </c>
+      <c r="P4" s="15"/>
       <c r="Q4" s="15">
-        <v>570.96774193548299</v>
-      </c>
-      <c r="R4" s="15"/>
-      <c r="S4" s="14">
-        <v>15</v>
-      </c>
+        <v>18.947368421052602</v>
+      </c>
+      <c r="R4" s="15">
+        <v>518.43317972350201</v>
+      </c>
+      <c r="S4" s="15"/>
       <c r="T4" s="14">
-        <v>675.86206896551698</v>
-      </c>
-      <c r="U4" s="15"/>
-      <c r="V4" s="15">
+        <v>16.6666666666666</v>
+      </c>
+      <c r="U4" s="14">
+        <v>626.896551724137</v>
+      </c>
+      <c r="V4" s="15"/>
+      <c r="W4" s="15">
         <v>18.947368421052602</v>
       </c>
-      <c r="W4" s="15">
-        <v>518.43317972350201</v>
-      </c>
-      <c r="X4" s="15"/>
-      <c r="Y4" s="14">
-        <v>16.6666666666666</v>
-      </c>
+      <c r="X4" s="15">
+        <v>539.17050691244197</v>
+      </c>
+      <c r="Y4" s="15"/>
       <c r="Z4" s="14">
-        <v>626.896551724137</v>
-      </c>
-      <c r="AA4" s="15"/>
-      <c r="AB4" s="15">
-        <v>18.947368421052602</v>
-      </c>
+        <v>14.4444444444444</v>
+      </c>
+      <c r="AA4" s="14">
+        <v>650.34482758620595</v>
+      </c>
+      <c r="AB4" s="15"/>
       <c r="AC4" s="15">
-        <v>539.17050691244197</v>
-      </c>
-      <c r="AD4" s="15"/>
-      <c r="AE4" s="14">
-        <v>14.4444444444444</v>
-      </c>
+        <v>11.052631578947301</v>
+      </c>
+      <c r="AD4" s="15">
+        <v>529.49308755760296</v>
+      </c>
+      <c r="AE4" s="15"/>
       <c r="AF4" s="14">
-        <v>650.34482758620595</v>
-      </c>
-      <c r="AG4" s="15"/>
-      <c r="AH4" s="15">
-        <v>11.052631578947301</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="AG4" s="14">
+        <v>631.03448275862002</v>
+      </c>
+      <c r="AH4" s="15"/>
       <c r="AI4" s="15">
-        <v>529.49308755760296</v>
-      </c>
-      <c r="AJ4" s="15"/>
-      <c r="AK4" s="14">
-        <v>5</v>
-      </c>
+        <v>17.8947368421052</v>
+      </c>
+      <c r="AJ4" s="15">
+        <v>495.62211981566799</v>
+      </c>
+      <c r="AK4" s="15"/>
       <c r="AL4" s="14">
-        <v>631.03448275862002</v>
-      </c>
-      <c r="AM4" s="15"/>
-      <c r="AN4" s="15">
-        <v>17.8947368421052</v>
-      </c>
+        <v>5.55555555555555</v>
+      </c>
+      <c r="AM4" s="14">
+        <v>619.31034482758605</v>
+      </c>
+      <c r="AN4" s="15"/>
       <c r="AO4" s="15">
-        <v>495.62211981566799</v>
-      </c>
-      <c r="AP4" s="15"/>
-      <c r="AQ4" s="14">
-        <v>5.55555555555555</v>
-      </c>
+        <v>19.4444444444444</v>
+      </c>
+      <c r="AP4" s="15">
+        <v>549.30555555555497</v>
+      </c>
+      <c r="AQ4" s="15"/>
       <c r="AR4" s="14">
-        <v>619.31034482758605</v>
-      </c>
-      <c r="AS4" s="15"/>
-      <c r="AT4" s="15">
-        <v>19.4444444444444</v>
-      </c>
+        <v>18.3333333333333</v>
+      </c>
+      <c r="AS4" s="14">
+        <v>662.23776223776201</v>
+      </c>
+      <c r="AT4" s="15"/>
       <c r="AU4" s="15">
-        <v>549.30555555555497</v>
-      </c>
-      <c r="AV4" s="15"/>
-      <c r="AW4" s="14">
-        <v>18.3333333333333</v>
-      </c>
+        <v>18.8888888888888</v>
+      </c>
+      <c r="AV4" s="15">
+        <v>536.11111111111097</v>
+      </c>
+      <c r="AW4" s="15"/>
       <c r="AX4" s="14">
-        <v>662.23776223776201</v>
-      </c>
-      <c r="AY4" s="15"/>
-      <c r="AZ4" s="15">
-        <v>18.8888888888888</v>
-      </c>
+        <v>7.7777777777777697</v>
+      </c>
+      <c r="AY4" s="14">
+        <v>660.83916083915994</v>
+      </c>
+      <c r="AZ4" s="15"/>
       <c r="BA4" s="15">
-        <v>536.11111111111097</v>
-      </c>
-      <c r="BB4" s="15"/>
-      <c r="BC4" s="14">
-        <v>7.7777777777777697</v>
-      </c>
+        <v>28.3333333333333</v>
+      </c>
+      <c r="BB4" s="15">
+        <v>509.722222222222</v>
+      </c>
+      <c r="BC4" s="15"/>
       <c r="BD4" s="14">
-        <v>660.83916083915994</v>
-      </c>
-      <c r="BE4" s="15"/>
-      <c r="BF4" s="15">
-        <v>28.3333333333333</v>
-      </c>
-      <c r="BG4" s="15">
-        <v>509.722222222222</v>
-      </c>
-      <c r="BH4" s="15"/>
-      <c r="BI4" s="14">
         <v>27.7777777777777</v>
       </c>
-      <c r="BJ4" s="14">
+      <c r="BE4" s="14">
         <v>621.67832167832103</v>
       </c>
     </row>
-    <row r="5" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:147" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>50</v>
       </c>
       <c r="B5" s="8">
         <v>525.368139223561</v>
       </c>
+      <c r="C5" s="2">
+        <v>100</v>
+      </c>
       <c r="D5" s="2">
+        <v>476.28519999999997</v>
+      </c>
+      <c r="E5" s="2">
         <v>100</v>
       </c>
-      <c r="E5" s="2">
-        <v>476.28519999999997</v>
+      <c r="F5" s="2">
+        <v>593.93268</v>
       </c>
       <c r="G5" s="2">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="H5" s="2">
-        <v>593.93268</v>
+        <v>727</v>
+      </c>
+      <c r="I5" s="2">
+        <v>300</v>
       </c>
       <c r="J5" s="2">
-        <v>300</v>
-      </c>
-      <c r="K5" s="2">
-        <v>727</v>
-      </c>
-      <c r="M5" s="2">
-        <v>300</v>
-      </c>
-      <c r="N5" s="2">
         <v>913</v>
       </c>
-      <c r="P5" s="15">
+      <c r="K5" s="15">
         <v>300.76219512195098</v>
       </c>
+      <c r="L5" s="15">
+        <v>476.30662020905902</v>
+      </c>
+      <c r="M5" s="15"/>
+      <c r="N5" s="14">
+        <v>298.01829268292602</v>
+      </c>
+      <c r="O5" s="14">
+        <v>544.90934449093402</v>
+      </c>
+      <c r="P5" s="15"/>
       <c r="Q5" s="15">
-        <v>476.30662020905902</v>
-      </c>
-      <c r="R5" s="15"/>
-      <c r="S5" s="14">
-        <v>298.01829268292602</v>
-      </c>
+        <v>300.076219512195</v>
+      </c>
+      <c r="R5" s="15">
+        <v>456.79442508710798</v>
+      </c>
+      <c r="S5" s="15"/>
       <c r="T5" s="14">
-        <v>544.90934449093402</v>
-      </c>
-      <c r="U5" s="15"/>
-      <c r="V5" s="15">
-        <v>300.076219512195</v>
-      </c>
+        <v>295.960365853658</v>
+      </c>
+      <c r="U5" s="14">
+        <v>519.80474198047398</v>
+      </c>
+      <c r="V5" s="15"/>
       <c r="W5" s="15">
-        <v>456.79442508710798</v>
-      </c>
-      <c r="X5" s="15"/>
-      <c r="Y5" s="14">
-        <v>295.960365853658</v>
-      </c>
+        <v>308.30792682926801</v>
+      </c>
+      <c r="X5" s="15">
+        <v>465.15679442508701</v>
+      </c>
+      <c r="Y5" s="15"/>
       <c r="Z5" s="14">
-        <v>519.80474198047398</v>
-      </c>
-      <c r="AA5" s="15"/>
-      <c r="AB5" s="15">
-        <v>308.30792682926801</v>
-      </c>
+        <v>294.58841463414598</v>
+      </c>
+      <c r="AA5" s="14">
+        <v>530.26499302649904</v>
+      </c>
+      <c r="AB5" s="15"/>
       <c r="AC5" s="15">
-        <v>465.15679442508701</v>
-      </c>
-      <c r="AD5" s="15"/>
-      <c r="AE5" s="14">
-        <v>294.58841463414598</v>
-      </c>
+        <v>287.72865853658499</v>
+      </c>
+      <c r="AD5" s="15">
+        <v>463.76306620208999</v>
+      </c>
+      <c r="AE5" s="15"/>
       <c r="AF5" s="14">
-        <v>530.26499302649904</v>
-      </c>
-      <c r="AG5" s="15"/>
-      <c r="AH5" s="15">
-        <v>287.72865853658499</v>
-      </c>
+        <v>303.50609756097498</v>
+      </c>
+      <c r="AG5" s="14">
+        <v>526.77824267782398</v>
+      </c>
+      <c r="AH5" s="15"/>
       <c r="AI5" s="15">
-        <v>463.76306620208999</v>
-      </c>
-      <c r="AJ5" s="15"/>
-      <c r="AK5" s="14">
-        <v>303.50609756097498</v>
-      </c>
+        <v>301.44817073170702</v>
+      </c>
+      <c r="AJ5" s="15">
+        <v>435.88850174215997</v>
+      </c>
+      <c r="AK5" s="15"/>
       <c r="AL5" s="14">
-        <v>526.77824267782398</v>
-      </c>
-      <c r="AM5" s="15"/>
-      <c r="AN5" s="15">
-        <v>301.44817073170702</v>
-      </c>
+        <v>300.76219512195098</v>
+      </c>
+      <c r="AM5" s="14">
+        <v>512.13389121338901</v>
+      </c>
+      <c r="AN5" s="15"/>
       <c r="AO5" s="15">
-        <v>435.88850174215997</v>
-      </c>
-      <c r="AP5" s="15"/>
-      <c r="AQ5" s="14">
-        <v>300.76219512195098</v>
-      </c>
+        <v>309.95405819295502</v>
+      </c>
+      <c r="AP5" s="15">
+        <v>469.06854130052699</v>
+      </c>
+      <c r="AQ5" s="15"/>
       <c r="AR5" s="14">
-        <v>512.13389121338901</v>
-      </c>
-      <c r="AS5" s="15"/>
-      <c r="AT5" s="15">
-        <v>309.95405819295502</v>
-      </c>
+        <v>298.853211009174</v>
+      </c>
+      <c r="AS5" s="14">
+        <v>531.40028288543101</v>
+      </c>
+      <c r="AT5" s="15"/>
       <c r="AU5" s="15">
-        <v>469.06854130052699</v>
-      </c>
-      <c r="AV5" s="15"/>
-      <c r="AW5" s="14">
-        <v>298.853211009174</v>
-      </c>
+        <v>385.068912710566</v>
+      </c>
+      <c r="AV5" s="15">
+        <v>450.08787346221402</v>
+      </c>
+      <c r="AW5" s="15"/>
       <c r="AX5" s="14">
-        <v>531.40028288543101</v>
-      </c>
-      <c r="AY5" s="15"/>
-      <c r="AZ5" s="15">
-        <v>385.068912710566</v>
-      </c>
+        <v>384.86238532110002</v>
+      </c>
+      <c r="AY5" s="14">
+        <v>500.99009900990097</v>
+      </c>
+      <c r="AZ5" s="15"/>
       <c r="BA5" s="15">
-        <v>450.08787346221402</v>
-      </c>
-      <c r="BB5" s="15"/>
-      <c r="BC5" s="14">
-        <v>384.86238532110002</v>
-      </c>
+        <v>298.92802450229698</v>
+      </c>
+      <c r="BB5" s="15">
+        <v>438.84007029876898</v>
+      </c>
+      <c r="BC5" s="15"/>
       <c r="BD5" s="14">
-        <v>500.99009900990097</v>
-      </c>
-      <c r="BE5" s="15"/>
-      <c r="BF5" s="15">
-        <v>298.92802450229698</v>
-      </c>
-      <c r="BG5" s="15">
-        <v>438.84007029876898</v>
-      </c>
-      <c r="BH5" s="15"/>
-      <c r="BI5" s="14">
         <v>297.47706422018302</v>
       </c>
-      <c r="BJ5" s="14">
+      <c r="BE5" s="14">
         <v>505.233380480905</v>
       </c>
     </row>
-    <row r="6" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:147" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>100</v>
       </c>
       <c r="B6" s="8">
         <v>508.76840696117802</v>
       </c>
+      <c r="C6" s="2">
+        <v>150</v>
+      </c>
       <c r="D6" s="2">
+        <v>461.81124999999997</v>
+      </c>
+      <c r="E6" s="2">
         <v>150</v>
       </c>
-      <c r="E6" s="2">
-        <v>461.81124999999997</v>
+      <c r="F6" s="2">
+        <v>570.30980999999997</v>
       </c>
       <c r="G6" s="2">
-        <v>150</v>
+        <v>400</v>
       </c>
       <c r="H6" s="2">
-        <v>570.30980999999997</v>
+        <v>741</v>
+      </c>
+      <c r="I6" s="2">
+        <v>400</v>
       </c>
       <c r="J6" s="2">
-        <v>400</v>
-      </c>
-      <c r="K6" s="2">
-        <v>741</v>
-      </c>
-      <c r="M6" s="2">
-        <v>400</v>
-      </c>
-      <c r="N6" s="2">
         <v>840</v>
       </c>
-      <c r="P6" s="15">
+      <c r="K6" s="15">
         <v>400.22865853658499</v>
       </c>
+      <c r="L6" s="15">
+        <v>454.70383275261298</v>
+      </c>
+      <c r="M6" s="15"/>
+      <c r="N6" s="14">
+        <v>398.17073170731697</v>
+      </c>
+      <c r="O6" s="14">
+        <v>502.37099023709902</v>
+      </c>
+      <c r="P6" s="15"/>
       <c r="Q6" s="15">
-        <v>454.70383275261298</v>
-      </c>
-      <c r="R6" s="15"/>
-      <c r="S6" s="14">
-        <v>398.17073170731697</v>
-      </c>
+        <v>400.22865853658499</v>
+      </c>
+      <c r="R6" s="15">
+        <v>443.55400696864098</v>
+      </c>
+      <c r="S6" s="15"/>
       <c r="T6" s="14">
-        <v>502.37099023709902</v>
-      </c>
-      <c r="U6" s="15"/>
-      <c r="V6" s="15">
+        <v>396.112804878048</v>
+      </c>
+      <c r="U6" s="14">
+        <v>489.12133891213301</v>
+      </c>
+      <c r="V6" s="15"/>
+      <c r="W6" s="15">
+        <v>391.31097560975599</v>
+      </c>
+      <c r="X6" s="15">
+        <v>437.28222996515598</v>
+      </c>
+      <c r="Y6" s="15"/>
+      <c r="Z6" s="14">
+        <v>405.71646341463401</v>
+      </c>
+      <c r="AA6" s="14">
+        <v>494.002789400278</v>
+      </c>
+      <c r="AB6" s="15"/>
+      <c r="AC6" s="15">
+        <v>406.40243902438999</v>
+      </c>
+      <c r="AD6" s="15">
+        <v>435.191637630662</v>
+      </c>
+      <c r="AE6" s="15"/>
+      <c r="AF6" s="14">
         <v>400.22865853658499</v>
       </c>
-      <c r="W6" s="15">
-        <v>443.55400696864098</v>
-      </c>
-      <c r="X6" s="15"/>
-      <c r="Y6" s="14">
-        <v>396.112804878048</v>
-      </c>
-      <c r="Z6" s="14">
-        <v>489.12133891213301</v>
-      </c>
-      <c r="AA6" s="15"/>
-      <c r="AB6" s="15">
-        <v>391.31097560975599</v>
-      </c>
-      <c r="AC6" s="15">
-        <v>437.28222996515598</v>
-      </c>
-      <c r="AD6" s="15"/>
-      <c r="AE6" s="14">
-        <v>405.71646341463401</v>
-      </c>
-      <c r="AF6" s="14">
-        <v>494.002789400278</v>
-      </c>
-      <c r="AG6" s="15"/>
-      <c r="AH6" s="15">
-        <v>406.40243902438999</v>
-      </c>
+      <c r="AG6" s="14">
+        <v>477.96373779637298</v>
+      </c>
+      <c r="AH6" s="15"/>
       <c r="AI6" s="15">
-        <v>435.191637630662</v>
-      </c>
-      <c r="AJ6" s="15"/>
-      <c r="AK6" s="14">
-        <v>400.22865853658499</v>
-      </c>
+        <v>400.91463414634097</v>
+      </c>
+      <c r="AJ6" s="15">
+        <v>410.10452961672399</v>
+      </c>
+      <c r="AK6" s="15"/>
       <c r="AL6" s="14">
-        <v>477.96373779637298</v>
-      </c>
-      <c r="AM6" s="15"/>
-      <c r="AN6" s="15">
-        <v>400.91463414634097</v>
-      </c>
+        <v>388.56707317073102</v>
+      </c>
+      <c r="AM6" s="14">
+        <v>476.56903765690299</v>
+      </c>
+      <c r="AN6" s="15"/>
       <c r="AO6" s="15">
-        <v>410.10452961672399</v>
-      </c>
-      <c r="AP6" s="15"/>
-      <c r="AQ6" s="14">
-        <v>388.56707317073102</v>
-      </c>
+        <v>411.94486983154599</v>
+      </c>
+      <c r="AP6" s="15">
+        <v>452.899824253075</v>
+      </c>
+      <c r="AQ6" s="15"/>
       <c r="AR6" s="14">
-        <v>476.56903765690299</v>
-      </c>
-      <c r="AS6" s="15"/>
-      <c r="AT6" s="15">
-        <v>411.94486983154599</v>
-      </c>
+        <v>411.00917431192602</v>
+      </c>
+      <c r="AS6" s="14">
+        <v>498.86845827439799</v>
+      </c>
+      <c r="AT6" s="15"/>
       <c r="AU6" s="15">
-        <v>452.899824253075</v>
-      </c>
-      <c r="AV6" s="15"/>
-      <c r="AW6" s="14">
-        <v>411.00917431192602</v>
-      </c>
+        <v>489.816232771822</v>
+      </c>
+      <c r="AV6" s="15">
+        <v>398.06678383128298</v>
+      </c>
+      <c r="AW6" s="15"/>
       <c r="AX6" s="14">
-        <v>498.86845827439799</v>
-      </c>
-      <c r="AY6" s="15"/>
-      <c r="AZ6" s="15">
-        <v>489.816232771822</v>
-      </c>
+        <v>486.00917431192602</v>
+      </c>
+      <c r="AY6" s="14">
+        <v>424.61103253182398</v>
+      </c>
+      <c r="AZ6" s="15"/>
       <c r="BA6" s="15">
-        <v>398.06678383128298</v>
-      </c>
-      <c r="BB6" s="15"/>
-      <c r="BC6" s="14">
-        <v>486.00917431192602</v>
-      </c>
+        <v>398.16232771822303</v>
+      </c>
+      <c r="BB6" s="15">
+        <v>421.26537785588698</v>
+      </c>
+      <c r="BC6" s="15"/>
       <c r="BD6" s="14">
-        <v>424.61103253182398</v>
-      </c>
-      <c r="BE6" s="15"/>
-      <c r="BF6" s="15">
-        <v>398.16232771822303</v>
-      </c>
-      <c r="BG6" s="15">
-        <v>421.26537785588698</v>
-      </c>
-      <c r="BH6" s="15"/>
-      <c r="BI6" s="14">
         <v>398.62385321100902</v>
       </c>
-      <c r="BJ6" s="14">
+      <c r="BE6" s="14">
         <v>475.53041018387501</v>
       </c>
     </row>
-    <row r="7" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:147" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>150</v>
       </c>
       <c r="B7" s="8">
         <v>494.846050870147</v>
       </c>
+      <c r="C7" s="2">
+        <v>200</v>
+      </c>
       <c r="D7" s="2">
+        <v>452.56896</v>
+      </c>
+      <c r="E7" s="2">
         <v>200</v>
       </c>
-      <c r="E7" s="2">
-        <v>452.56896</v>
+      <c r="F7" s="2">
+        <v>551.91571999999996</v>
       </c>
       <c r="G7" s="2">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="H7" s="2">
-        <v>551.91571999999996</v>
+        <v>537</v>
+      </c>
+      <c r="I7" s="2">
+        <v>500</v>
       </c>
       <c r="J7" s="2">
-        <v>500</v>
-      </c>
-      <c r="K7" s="2">
-        <v>537</v>
-      </c>
-      <c r="M7" s="2">
-        <v>500</v>
-      </c>
-      <c r="N7" s="2">
         <v>685</v>
       </c>
-      <c r="P7" s="15">
+      <c r="K7" s="15">
         <v>502.43902439024299</v>
       </c>
+      <c r="L7" s="15">
+        <v>405.92334494773502</v>
+      </c>
+      <c r="M7" s="15"/>
+      <c r="N7" s="14">
+        <v>498.32317073170702</v>
+      </c>
+      <c r="O7" s="14">
+        <v>423.57043235704299</v>
+      </c>
+      <c r="P7" s="15"/>
       <c r="Q7" s="15">
-        <v>405.92334494773502</v>
-      </c>
-      <c r="R7" s="15"/>
-      <c r="S7" s="14">
-        <v>498.32317073170702</v>
-      </c>
+        <v>502.43902439024299</v>
+      </c>
+      <c r="R7" s="15">
+        <v>389.19860627177701</v>
+      </c>
+      <c r="S7" s="15"/>
       <c r="T7" s="14">
-        <v>423.57043235704299</v>
-      </c>
-      <c r="U7" s="15"/>
-      <c r="V7" s="15">
-        <v>502.43902439024299</v>
-      </c>
+        <v>496.26524390243901</v>
+      </c>
+      <c r="U7" s="14">
+        <v>410.320781032078</v>
+      </c>
+      <c r="V7" s="15"/>
       <c r="W7" s="15">
-        <v>389.19860627177701</v>
-      </c>
-      <c r="X7" s="15"/>
-      <c r="Y7" s="14">
-        <v>496.26524390243901</v>
-      </c>
+        <v>493.52134146341399</v>
+      </c>
+      <c r="X7" s="15">
+        <v>396.86411149825699</v>
+      </c>
+      <c r="Y7" s="15"/>
       <c r="Z7" s="14">
+        <v>507.24085365853603</v>
+      </c>
+      <c r="AA7" s="14">
+        <v>415.20223152022299</v>
+      </c>
+      <c r="AB7" s="15"/>
+      <c r="AC7" s="15">
+        <v>515.47256097560899</v>
+      </c>
+      <c r="AD7" s="15">
+        <v>393.37979094076599</v>
+      </c>
+      <c r="AE7" s="15"/>
+      <c r="AF7" s="14">
+        <v>484.60365853658499</v>
+      </c>
+      <c r="AG7" s="14">
         <v>410.320781032078</v>
       </c>
-      <c r="AA7" s="15"/>
-      <c r="AB7" s="15">
-        <v>493.52134146341399</v>
-      </c>
-      <c r="AC7" s="15">
-        <v>396.86411149825699</v>
-      </c>
-      <c r="AD7" s="15"/>
-      <c r="AE7" s="14">
-        <v>507.24085365853603</v>
-      </c>
-      <c r="AF7" s="14">
-        <v>415.20223152022299</v>
-      </c>
-      <c r="AG7" s="15"/>
-      <c r="AH7" s="15">
-        <v>515.47256097560899</v>
-      </c>
+      <c r="AH7" s="15"/>
       <c r="AI7" s="15">
-        <v>393.37979094076599</v>
-      </c>
-      <c r="AJ7" s="15"/>
-      <c r="AK7" s="14">
-        <v>484.60365853658499</v>
-      </c>
+        <v>504.49695121951203</v>
+      </c>
+      <c r="AJ7" s="15">
+        <v>375.95818815331</v>
+      </c>
+      <c r="AK7" s="15"/>
       <c r="AL7" s="14">
-        <v>410.320781032078</v>
-      </c>
-      <c r="AM7" s="15"/>
-      <c r="AN7" s="15">
-        <v>504.49695121951203</v>
-      </c>
+        <v>492.835365853658</v>
+      </c>
+      <c r="AM7" s="14">
+        <v>399.860529986053</v>
+      </c>
+      <c r="AN7" s="15"/>
       <c r="AO7" s="15">
-        <v>375.95818815331</v>
-      </c>
-      <c r="AP7" s="15"/>
-      <c r="AQ7" s="14">
-        <v>492.835365853658</v>
-      </c>
+        <v>509.80091883614</v>
+      </c>
+      <c r="AP7" s="15">
+        <v>400.87873462214401</v>
+      </c>
+      <c r="AQ7" s="15"/>
       <c r="AR7" s="14">
-        <v>399.860529986053</v>
-      </c>
-      <c r="AS7" s="15"/>
-      <c r="AT7" s="15">
-        <v>509.80091883614</v>
-      </c>
-      <c r="AU7" s="15">
-        <v>400.87873462214401</v>
-      </c>
+        <v>509.40366972477</v>
+      </c>
+      <c r="AS7" s="14">
+        <v>419.660537482319</v>
+      </c>
+      <c r="AT7" s="15"/>
+      <c r="AU7" s="15"/>
       <c r="AV7" s="15"/>
-      <c r="AW7" s="14">
-        <v>509.40366972477</v>
-      </c>
-      <c r="AX7" s="14">
-        <v>419.660537482319</v>
-      </c>
+      <c r="AW7" s="15"/>
+      <c r="AX7" s="15"/>
       <c r="AY7" s="15"/>
       <c r="AZ7" s="15"/>
-      <c r="BA7" s="15"/>
-      <c r="BB7" s="15"/>
+      <c r="BA7" s="15">
+        <v>509.11179173047401</v>
+      </c>
+      <c r="BB7" s="15">
+        <v>380.49209138840001</v>
+      </c>
       <c r="BC7" s="15"/>
-      <c r="BD7" s="15"/>
-      <c r="BE7" s="15"/>
-      <c r="BF7" s="15">
-        <v>509.11179173047401</v>
-      </c>
-      <c r="BG7" s="15">
-        <v>380.49209138840001</v>
-      </c>
-      <c r="BH7" s="15"/>
-      <c r="BI7" s="14">
+      <c r="BD7" s="14">
         <v>510.09174311926603</v>
       </c>
-      <c r="BJ7" s="14">
+      <c r="BE7" s="14">
         <v>399.15134370579898</v>
       </c>
     </row>
-    <row r="8" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:147" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>200</v>
       </c>
       <c r="B8" s="8">
         <v>486.27844712182002</v>
       </c>
+      <c r="C8" s="2">
+        <v>250</v>
+      </c>
       <c r="D8" s="2">
+        <v>445.93817999999999</v>
+      </c>
+      <c r="E8" s="2">
         <v>250</v>
       </c>
-      <c r="E8" s="2">
-        <v>445.93817999999999</v>
+      <c r="F8" s="2">
+        <v>534.82883000000004</v>
       </c>
       <c r="G8" s="2">
-        <v>250</v>
+        <v>600</v>
       </c>
       <c r="H8" s="2">
-        <v>534.82883000000004</v>
+        <v>330</v>
+      </c>
+      <c r="I8" s="2">
+        <v>600</v>
       </c>
       <c r="J8" s="2">
-        <v>600</v>
-      </c>
-      <c r="K8" s="2">
-        <v>330</v>
-      </c>
-      <c r="M8" s="2">
-        <v>600</v>
-      </c>
-      <c r="N8" s="2">
         <v>428</v>
       </c>
-      <c r="P8" s="15">
+      <c r="K8" s="15">
         <v>604.64939024390196</v>
       </c>
+      <c r="L8" s="15">
+        <v>283.97212543554002</v>
+      </c>
+      <c r="M8" s="15"/>
+      <c r="N8" s="14">
+        <v>598.47560975609701</v>
+      </c>
+      <c r="O8" s="14">
+        <v>292.46861924686198</v>
+      </c>
+      <c r="P8" s="15"/>
       <c r="Q8" s="15">
-        <v>283.97212543554002</v>
-      </c>
-      <c r="R8" s="15"/>
-      <c r="S8" s="14">
-        <v>598.47560975609701</v>
-      </c>
+        <v>603.96341463414603</v>
+      </c>
+      <c r="R8" s="15">
+        <v>274.91289198606199</v>
+      </c>
+      <c r="S8" s="15"/>
       <c r="T8" s="14">
-        <v>292.46861924686198</v>
-      </c>
-      <c r="U8" s="15"/>
-      <c r="V8" s="15">
-        <v>603.96341463414603</v>
-      </c>
+        <v>597.78963414634097</v>
+      </c>
+      <c r="U8" s="14">
+        <v>282.008368200836</v>
+      </c>
+      <c r="V8" s="15"/>
       <c r="W8" s="15">
-        <v>274.91289198606199</v>
-      </c>
-      <c r="X8" s="15"/>
-      <c r="Y8" s="14">
-        <v>597.78963414634097</v>
-      </c>
+        <v>616.99695121951197</v>
+      </c>
+      <c r="X8" s="15">
+        <v>277.70034843205502</v>
+      </c>
+      <c r="Y8" s="15"/>
       <c r="Z8" s="14">
-        <v>282.008368200836</v>
-      </c>
-      <c r="AA8" s="15"/>
-      <c r="AB8" s="15">
-        <v>616.99695121951197</v>
-      </c>
+        <v>608.76524390243901</v>
+      </c>
+      <c r="AA8" s="14">
+        <v>288.98186889818601</v>
+      </c>
+      <c r="AB8" s="15"/>
       <c r="AC8" s="15">
+        <v>592.30182926829195</v>
+      </c>
+      <c r="AD8" s="15">
         <v>277.70034843205502</v>
       </c>
-      <c r="AD8" s="15"/>
-      <c r="AE8" s="14">
-        <v>608.76524390243901</v>
-      </c>
+      <c r="AE8" s="15"/>
       <c r="AF8" s="14">
-        <v>288.98186889818601</v>
-      </c>
-      <c r="AG8" s="15"/>
-      <c r="AH8" s="15">
-        <v>592.30182926829195</v>
-      </c>
+        <v>608.07926829268297</v>
+      </c>
+      <c r="AG8" s="14">
+        <v>279.21896792189602</v>
+      </c>
+      <c r="AH8" s="15"/>
       <c r="AI8" s="15">
-        <v>277.70034843205502</v>
-      </c>
-      <c r="AJ8" s="15"/>
-      <c r="AK8" s="14">
-        <v>608.07926829268297</v>
-      </c>
+        <v>606.02134146341405</v>
+      </c>
+      <c r="AJ8" s="15">
+        <v>257.49128919860601</v>
+      </c>
+      <c r="AK8" s="15"/>
       <c r="AL8" s="14">
-        <v>279.21896792189602</v>
-      </c>
-      <c r="AM8" s="15"/>
-      <c r="AN8" s="15">
-        <v>606.02134146341405</v>
-      </c>
+        <v>601.90548780487802</v>
+      </c>
+      <c r="AM8" s="14">
+        <v>270.15341701534101</v>
+      </c>
+      <c r="AN8" s="15"/>
       <c r="AO8" s="15">
-        <v>257.49128919860601</v>
-      </c>
-      <c r="AP8" s="15"/>
-      <c r="AQ8" s="14">
-        <v>601.90548780487802</v>
-      </c>
+        <v>613.16998468606403</v>
+      </c>
+      <c r="AP8" s="15">
+        <v>284.18277680140602</v>
+      </c>
+      <c r="AQ8" s="15"/>
       <c r="AR8" s="14">
-        <v>270.15341701534101</v>
-      </c>
-      <c r="AS8" s="15"/>
-      <c r="AT8" s="15">
-        <v>613.16998468606403</v>
-      </c>
-      <c r="AU8" s="15">
-        <v>284.18277680140602</v>
-      </c>
+        <v>609.86238532109996</v>
+      </c>
+      <c r="AS8" s="14">
+        <v>295.89816124469502</v>
+      </c>
+      <c r="AT8" s="15"/>
+      <c r="AU8" s="15"/>
       <c r="AV8" s="15"/>
-      <c r="AW8" s="14">
-        <v>609.86238532109996</v>
-      </c>
-      <c r="AX8" s="14">
-        <v>295.89816124469502</v>
-      </c>
+      <c r="AW8" s="15"/>
+      <c r="AX8" s="15"/>
       <c r="AY8" s="15"/>
       <c r="AZ8" s="15"/>
-      <c r="BA8" s="15"/>
-      <c r="BB8" s="15"/>
+      <c r="BA8" s="15">
+        <v>613.16998468606403</v>
+      </c>
+      <c r="BB8" s="15">
+        <v>270.1230228471</v>
+      </c>
       <c r="BC8" s="15"/>
-      <c r="BD8" s="15"/>
-      <c r="BE8" s="15"/>
-      <c r="BF8" s="15">
-        <v>613.16998468606403</v>
-      </c>
-      <c r="BG8" s="15">
-        <v>270.1230228471</v>
-      </c>
-      <c r="BH8" s="15"/>
-      <c r="BI8" s="14">
+      <c r="BD8" s="14">
         <v>609.17431192660501</v>
       </c>
-      <c r="BJ8" s="14">
+      <c r="BE8" s="14">
         <v>282.46110325318199</v>
       </c>
     </row>
-    <row r="9" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:147" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>250</v>
       </c>
       <c r="B9" s="8">
         <v>479.31726907630502</v>
       </c>
+      <c r="C9" s="2">
+        <v>300</v>
+      </c>
       <c r="D9" s="2">
+        <v>436.69731999999999</v>
+      </c>
+      <c r="E9" s="2">
         <v>300</v>
       </c>
-      <c r="E9" s="2">
-        <v>436.69731999999999</v>
+      <c r="F9" s="2">
+        <v>515.12753999999995</v>
       </c>
       <c r="G9" s="2">
-        <v>300</v>
+        <v>700</v>
       </c>
       <c r="H9" s="2">
-        <v>515.12753999999995</v>
+        <v>163</v>
+      </c>
+      <c r="I9" s="2">
+        <v>700</v>
       </c>
       <c r="J9" s="2">
-        <v>700</v>
-      </c>
-      <c r="K9" s="2">
-        <v>163</v>
-      </c>
-      <c r="M9" s="2">
-        <v>700</v>
-      </c>
-      <c r="N9" s="2">
         <v>247</v>
       </c>
-      <c r="P9" s="15">
+      <c r="K9" s="15">
         <v>703.42987804877998</v>
       </c>
-      <c r="Q9" s="15">
+      <c r="L9" s="15">
         <v>132.75261324041799</v>
       </c>
+      <c r="M9" s="15"/>
+      <c r="N9" s="14">
+        <v>699.31402439024396</v>
+      </c>
+      <c r="O9" s="14">
+        <v>159.27475592747501</v>
+      </c>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
       <c r="R9" s="15"/>
-      <c r="S9" s="14">
-        <v>699.31402439024396</v>
-      </c>
-      <c r="T9" s="14">
-        <v>159.27475592747501</v>
-      </c>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15"/>
       <c r="U9" s="15"/>
       <c r="V9" s="15"/>
       <c r="W9" s="15"/>
@@ -3646,173 +4237,168 @@
       <c r="BC9" s="15"/>
       <c r="BD9" s="15"/>
       <c r="BE9" s="15"/>
-      <c r="BF9" s="15"/>
-      <c r="BG9" s="15"/>
-      <c r="BH9" s="15"/>
-      <c r="BI9" s="15"/>
-      <c r="BJ9" s="15"/>
-    </row>
-    <row r="10" spans="1:62" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:147" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>300</v>
       </c>
       <c r="B10" s="8">
         <v>471.82061579651901</v>
       </c>
+      <c r="C10" s="2">
+        <v>350</v>
+      </c>
       <c r="D10" s="2">
+        <v>427.45071999999999</v>
+      </c>
+      <c r="E10" s="2">
         <v>350</v>
       </c>
-      <c r="E10" s="2">
-        <v>427.45071999999999</v>
-      </c>
-      <c r="G10" s="2">
-        <v>350</v>
-      </c>
-      <c r="H10" s="2">
+      <c r="F10" s="2">
         <v>495.42626000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:147" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>350</v>
       </c>
       <c r="B11" s="8">
         <v>462.71753681392198</v>
       </c>
+      <c r="C11" s="2">
+        <v>400</v>
+      </c>
       <c r="D11" s="2">
+        <v>410.36381999999998</v>
+      </c>
+      <c r="E11" s="2">
         <v>400</v>
       </c>
-      <c r="E11" s="2">
-        <v>410.36381999999998</v>
-      </c>
-      <c r="G11" s="2">
-        <v>400</v>
-      </c>
-      <c r="H11" s="2">
+      <c r="F11" s="2">
         <v>466.57317999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:147" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>400</v>
       </c>
       <c r="B12" s="8">
         <v>448.79518072289102</v>
       </c>
+      <c r="C12" s="2">
+        <v>450</v>
+      </c>
       <c r="D12" s="2">
+        <v>388.04959000000002</v>
+      </c>
+      <c r="E12" s="2">
         <v>450</v>
       </c>
-      <c r="E12" s="2">
-        <v>388.04959000000002</v>
-      </c>
-      <c r="G12" s="2">
-        <v>450</v>
-      </c>
-      <c r="H12" s="2">
+      <c r="F12" s="2">
         <v>432.49275</v>
       </c>
     </row>
-    <row r="13" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:147" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>450</v>
       </c>
       <c r="B13" s="8">
         <v>427.376171352075</v>
       </c>
+      <c r="C13" s="2">
+        <v>500</v>
+      </c>
       <c r="D13" s="2">
+        <v>353.96629000000001</v>
+      </c>
+      <c r="E13" s="2">
         <v>500</v>
       </c>
-      <c r="E13" s="2">
-        <v>353.96629000000001</v>
-      </c>
-      <c r="G13" s="2">
-        <v>500</v>
-      </c>
-      <c r="H13" s="2">
+      <c r="F13" s="2">
         <v>389.26197000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:147" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>500</v>
       </c>
       <c r="B14" s="8">
         <v>397.92503346720201</v>
       </c>
+      <c r="C14" s="2">
+        <v>550</v>
+      </c>
       <c r="D14" s="2">
+        <v>310.73838999999998</v>
+      </c>
+      <c r="E14" s="2">
         <v>550</v>
       </c>
-      <c r="E14" s="2">
-        <v>310.73838999999998</v>
-      </c>
-      <c r="G14" s="2">
-        <v>550</v>
-      </c>
-      <c r="H14" s="2">
+      <c r="F14" s="2">
         <v>339.49808999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:147" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>550</v>
       </c>
       <c r="B15" s="8">
         <v>355.62248995983902</v>
       </c>
+      <c r="C15" s="2">
+        <v>600</v>
+      </c>
       <c r="D15" s="2">
+        <v>253.12702999999999</v>
+      </c>
+      <c r="E15" s="2">
         <v>600</v>
       </c>
-      <c r="E15" s="2">
-        <v>253.12702999999999</v>
-      </c>
-      <c r="G15" s="2">
-        <v>600</v>
-      </c>
-      <c r="H15" s="2">
+      <c r="F15" s="2">
         <v>276.65652999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:147" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>600</v>
       </c>
       <c r="B16" s="8">
         <v>299.93306559571602</v>
       </c>
+      <c r="C16" s="2">
+        <v>650</v>
+      </c>
       <c r="D16" s="2">
+        <v>178.52502999999999</v>
+      </c>
+      <c r="E16" s="2">
         <v>650</v>
       </c>
-      <c r="E16" s="2">
-        <v>178.52502999999999</v>
-      </c>
-      <c r="G16" s="2">
-        <v>650</v>
-      </c>
-      <c r="H16" s="2">
+      <c r="F16" s="2">
         <v>199.44013000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>650</v>
       </c>
       <c r="B17" s="8">
         <v>228.17938420348</v>
       </c>
+      <c r="C17" s="2">
+        <v>700</v>
+      </c>
       <c r="D17" s="2">
+        <v>81.697839999999999</v>
+      </c>
+      <c r="E17" s="2">
         <v>700</v>
       </c>
-      <c r="E17" s="2">
-        <v>81.697839999999999</v>
-      </c>
-      <c r="G17" s="2">
-        <v>700</v>
-      </c>
-      <c r="H17" s="2">
+      <c r="F17" s="2">
         <v>105.22734</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>700</v>
       </c>
@@ -3820,27 +4406,30 @@
         <v>137.14859437750999</v>
       </c>
     </row>
-    <row r="39" spans="1:62" ht="152.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:57" ht="152.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="16" t="s">
         <v>17</v>
       </c>
       <c r="B39" s="16"/>
-      <c r="E39" s="16" t="s">
+      <c r="D39" s="16" t="s">
         <v>40</v>
       </c>
+      <c r="E39" s="16"/>
       <c r="F39" s="16"/>
-      <c r="G39" s="16"/>
+      <c r="G39" s="16" t="s">
+        <v>65</v>
+      </c>
       <c r="H39" s="16"/>
-      <c r="J39" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="K39" s="16"/>
+      <c r="I39" s="16"/>
+      <c r="J39" s="16"/>
+      <c r="K39" s="16" t="s">
+        <v>57</v>
+      </c>
       <c r="L39" s="16"/>
       <c r="M39" s="16"/>
       <c r="N39" s="16"/>
-      <c r="P39" s="16" t="s">
-        <v>57</v>
-      </c>
+      <c r="O39" s="16"/>
+      <c r="P39" s="16"/>
       <c r="Q39" s="16"/>
       <c r="R39" s="16"/>
       <c r="S39" s="16"/>
@@ -3882,44 +4471,39 @@
       <c r="BC39" s="16"/>
       <c r="BD39" s="16"/>
       <c r="BE39" s="16"/>
-      <c r="BF39" s="16"/>
-      <c r="BG39" s="16"/>
-      <c r="BH39" s="16"/>
-      <c r="BI39" s="16"/>
-      <c r="BJ39" s="16"/>
-    </row>
-    <row r="40" spans="1:62" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="40" spans="1:57" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" s="7" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="BF1:BG1"/>
-    <mergeCell ref="BI1:BJ1"/>
+    <mergeCell ref="BA1:BB1"/>
+    <mergeCell ref="BD1:BE1"/>
     <mergeCell ref="A39:B39"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="J39:N39"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="G39:J39"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="P39:BJ39"/>
-    <mergeCell ref="E39:H39"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="AB1:AC1"/>
-    <mergeCell ref="AE1:AF1"/>
-    <mergeCell ref="AH1:AI1"/>
-    <mergeCell ref="AK1:AL1"/>
-    <mergeCell ref="AN1:AO1"/>
-    <mergeCell ref="AQ1:AR1"/>
-    <mergeCell ref="AT1:AU1"/>
-    <mergeCell ref="AW1:AX1"/>
-    <mergeCell ref="AZ1:BA1"/>
-    <mergeCell ref="BC1:BD1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="K39:BE39"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="AO1:AP1"/>
+    <mergeCell ref="AR1:AS1"/>
+    <mergeCell ref="AU1:AV1"/>
+    <mergeCell ref="AX1:AY1"/>
+    <mergeCell ref="Z1:AA1"/>
+    <mergeCell ref="AC1:AD1"/>
+    <mergeCell ref="AF1:AG1"/>
+    <mergeCell ref="AI1:AJ1"/>
+    <mergeCell ref="AL1:AM1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A40" r:id="rId1" xr:uid="{BD8505B1-6312-437D-81B2-778CAED7521D}"/>
@@ -3933,8 +4517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96129535-FEF3-45F0-8A22-F7741A343589}">
   <dimension ref="A1:U42"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4492,8 +5076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F380984-BC1C-4914-83CA-6C32A0D3A058}">
   <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36:N36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R3" sqref="R3:Z29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4996,7 +5580,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE9D7C7B-E4E9-42EA-9DB0-66C5C7498970}">
   <dimension ref="A1:W34"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M34" sqref="M34:N34"/>
     </sheetView>
   </sheetViews>
@@ -5455,7 +6039,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47A88C06-9205-4EF5-AC1B-94A0B27B9154}">
   <dimension ref="A1:T52"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="P52" sqref="P52:T52"/>
     </sheetView>
   </sheetViews>
@@ -6344,8 +6928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A8953B6-FF81-4C42-8C9F-1BD7638290AD}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6472,7 +7056,7 @@
   <dimension ref="A1:Y65"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50:F65"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6513,7 +7097,7 @@
         <v>448.39537869062798</v>
       </c>
       <c r="D4" s="2">
-        <f>F51+273</f>
+        <f t="shared" ref="D4:D18" si="0">F51+273</f>
         <v>293.54795000000001</v>
       </c>
       <c r="E4" s="2">
@@ -6528,7 +7112,7 @@
         <v>461.48908857509599</v>
       </c>
       <c r="D5" s="2">
-        <f>F52+273</f>
+        <f t="shared" si="0"/>
         <v>326.42466000000002</v>
       </c>
       <c r="E5" s="2">
@@ -6543,7 +7127,7 @@
         <v>475.35301668806102</v>
       </c>
       <c r="D6" s="2">
-        <f>F53+273</f>
+        <f t="shared" si="0"/>
         <v>373</v>
       </c>
       <c r="E6" s="2">
@@ -6558,7 +7142,7 @@
         <v>485.36585365853603</v>
       </c>
       <c r="D7" s="2">
-        <f>F54+273</f>
+        <f t="shared" si="0"/>
         <v>425.05479000000003</v>
       </c>
       <c r="E7" s="2">
@@ -6573,7 +7157,7 @@
         <v>496.14890885750901</v>
       </c>
       <c r="D8" s="2">
-        <f>F55+273</f>
+        <f t="shared" si="0"/>
         <v>474.36986000000002</v>
       </c>
       <c r="E8" s="2">
@@ -6588,7 +7172,7 @@
         <v>504.621309370988</v>
       </c>
       <c r="D9" s="2">
-        <f>F56+273</f>
+        <f t="shared" si="0"/>
         <v>523.68493000000001</v>
       </c>
       <c r="E9" s="2">
@@ -6603,7 +7187,7 @@
         <v>513.86392811296503</v>
       </c>
       <c r="D10" s="2">
-        <f>F57+273</f>
+        <f t="shared" si="0"/>
         <v>573</v>
       </c>
       <c r="E10" s="2">
@@ -6618,7 +7202,7 @@
         <v>521.56611039794598</v>
       </c>
       <c r="D11" s="2">
-        <f>F58+273</f>
+        <f t="shared" si="0"/>
         <v>622.31506999999999</v>
       </c>
       <c r="E11" s="2">
@@ -6633,7 +7217,7 @@
         <v>530.03851091142405</v>
       </c>
       <c r="D12" s="2">
-        <f>F59+273</f>
+        <f t="shared" si="0"/>
         <v>671.63013999999998</v>
       </c>
       <c r="E12" s="2">
@@ -6648,7 +7232,7 @@
         <v>536.97047496790697</v>
       </c>
       <c r="D13" s="2">
-        <f>F60+273</f>
+        <f t="shared" si="0"/>
         <v>723.68493000000001</v>
       </c>
       <c r="E13" s="2">
@@ -6663,7 +7247,7 @@
         <v>544.67265725288803</v>
       </c>
       <c r="D14" s="2">
-        <f>F61+273</f>
+        <f t="shared" si="0"/>
         <v>773</v>
       </c>
       <c r="E14" s="2">
@@ -6678,7 +7262,7 @@
         <v>550.83440308087199</v>
       </c>
       <c r="D15" s="2">
-        <f>F62+273</f>
+        <f t="shared" si="0"/>
         <v>822.31506999999999</v>
       </c>
       <c r="E15" s="2">
@@ -6693,7 +7277,7 @@
         <v>556.99614890885698</v>
       </c>
       <c r="D16" s="2">
-        <f>F63+273</f>
+        <f t="shared" si="0"/>
         <v>871.63013999999998</v>
       </c>
       <c r="E16" s="2">
@@ -6708,7 +7292,7 @@
         <v>565.46854942233597</v>
       </c>
       <c r="D17" s="2">
-        <f>F64+273</f>
+        <f t="shared" si="0"/>
         <v>920.94520999999997</v>
       </c>
       <c r="E17" s="2">
@@ -6723,7 +7307,7 @@
         <v>573.17073170731703</v>
       </c>
       <c r="D18" s="2">
-        <f>F65+273</f>
+        <f t="shared" si="0"/>
         <v>973</v>
       </c>
       <c r="E18" s="2">
@@ -6919,7 +7503,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D45C8D-0E1D-4271-9C84-7C91BB3EB92B}">
   <dimension ref="A1:V49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D5" sqref="D5:D16"/>
     </sheetView>
   </sheetViews>
@@ -7584,8 +8168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B73F6F46-AAA6-4839-9EF2-18966D033E04}">
   <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
plot single data sets or concatenated data
</commit_message>
<xml_diff>
--- a/Jupyter/Eurofer/Eurofer_data.xlsx
+++ b/Jupyter/Eurofer/Eurofer_data.xlsx
@@ -1,36 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Research\Repos\DatabaseCodes\Jupyter\Eurofer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5852CB07-8AC2-4253-A80D-3CE00E7CA3CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DF9356D-C07A-4E28-8100-243C35200E59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="852" activeTab="10" xr2:uid="{D289EE42-B074-4616-9B9B-4CE9F1662138}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="852" activeTab="7" xr2:uid="{D289EE42-B074-4616-9B9B-4CE9F1662138}"/>
   </bookViews>
   <sheets>
-    <sheet name="Eurofer_density" sheetId="15" r:id="rId1"/>
-    <sheet name="Eurofer_diffusivity" sheetId="1" r:id="rId2"/>
-    <sheet name="Eurofer_specific_heat" sheetId="3" r:id="rId3"/>
-    <sheet name="Eurofer_conductivity" sheetId="4" r:id="rId4"/>
-    <sheet name="Eurofer_resistivity" sheetId="5" r:id="rId5"/>
-    <sheet name="Eurofer_CTE" sheetId="6" r:id="rId6"/>
-    <sheet name="Eurofer_emissivity" sheetId="9" r:id="rId7"/>
-    <sheet name="Eurofer_elastic" sheetId="10" r:id="rId8"/>
-    <sheet name="Eurofer_hardness" sheetId="16" r:id="rId9"/>
-    <sheet name="Eurofer_strength" sheetId="7" r:id="rId10"/>
-    <sheet name="Eurofer_ductility" sheetId="8" r:id="rId11"/>
-    <sheet name="Eurofer_toughness" sheetId="14" r:id="rId12"/>
-    <sheet name="Eurofer_creep" sheetId="11" r:id="rId13"/>
-    <sheet name="Eurofer_fatigue" sheetId="12" r:id="rId14"/>
-    <sheet name="Eurofer_chemical" sheetId="13" r:id="rId15"/>
+    <sheet name="Density" sheetId="15" r:id="rId1"/>
+    <sheet name="Diffusivity" sheetId="1" r:id="rId2"/>
+    <sheet name="Specific Heat" sheetId="3" r:id="rId3"/>
+    <sheet name="Conductivity" sheetId="4" r:id="rId4"/>
+    <sheet name="Resistivity" sheetId="5" r:id="rId5"/>
+    <sheet name="CTE" sheetId="6" r:id="rId6"/>
+    <sheet name="Emissivity" sheetId="9" r:id="rId7"/>
+    <sheet name="Elastic Properties" sheetId="10" r:id="rId8"/>
+    <sheet name="Hardness" sheetId="16" r:id="rId9"/>
+    <sheet name="Strength" sheetId="7" r:id="rId10"/>
+    <sheet name="Ductility" sheetId="8" r:id="rId11"/>
+    <sheet name="Toughness" sheetId="14" r:id="rId12"/>
+    <sheet name="Creep" sheetId="11" r:id="rId13"/>
+    <sheet name="Fatigue" sheetId="12" r:id="rId14"/>
+    <sheet name="Chemical" sheetId="13" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -51,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="105">
   <si>
     <t>Temp (K)</t>
   </si>
@@ -498,9 +497,6 @@
     <t>Table. 6.Das, Aniruddh, et al. "Microstructure and fracture toughness characterization of three 9Cr ODS EUROFER steels with different thermo-mechanical treatments." Journal of Nuclear Materials 542 (2020): 152464.</t>
   </si>
   <si>
-    <t>Elastic Modulus (Gpa)</t>
-  </si>
-  <si>
     <t>Eurofer E</t>
   </si>
   <si>
@@ -621,6 +617,32 @@
   </si>
   <si>
     <t>Temp(K)</t>
+  </si>
+  <si>
+    <r>
+      <t>Temp (K</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Eurofer G</t>
+  </si>
+  <si>
+    <t>G (Gpa)</t>
+  </si>
+  <si>
+    <t>E (Gpa)</t>
+  </si>
+  <si>
+    <t>Note: No specific data for Eurofer were found.  F82H data are used.</t>
   </si>
 </sst>
 </file>
@@ -1842,16 +1864,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>289879</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>73979</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>2235200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1874,8 +1896,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="2857500"/>
-          <a:ext cx="3585529" cy="2152650"/>
+          <a:off x="2990850" y="5308600"/>
+          <a:ext cx="3750629" cy="2082800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2512,7 +2534,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -2663,75 +2685,75 @@
       </c>
       <c r="J1" s="16"/>
       <c r="K1" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L1" s="16"/>
       <c r="M1" s="11"/>
       <c r="N1" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O1" s="16"/>
       <c r="Q1" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="R1" s="16"/>
       <c r="S1" s="11"/>
       <c r="T1" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="U1" s="16"/>
       <c r="W1" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="X1" s="16"/>
       <c r="Y1" s="11"/>
       <c r="Z1" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AA1" s="16"/>
       <c r="AC1" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AD1" s="16"/>
       <c r="AE1" s="11"/>
       <c r="AF1" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AG1" s="16"/>
       <c r="AI1" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AJ1" s="16"/>
       <c r="AK1" s="11"/>
       <c r="AL1" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AM1" s="16"/>
       <c r="AO1" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AP1" s="16"/>
       <c r="AQ1" s="11"/>
       <c r="AR1" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AS1" s="16"/>
       <c r="AU1" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AV1" s="16"/>
       <c r="AW1" s="11"/>
       <c r="AX1" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AY1" s="16"/>
       <c r="BA1" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="BB1" s="16"/>
       <c r="BC1" s="11"/>
       <c r="BD1" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="BE1" s="16"/>
     </row>
@@ -3368,7 +3390,7 @@
         <v>56</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="R3" s="2" t="s">
         <v>16</v>
@@ -4479,6 +4501,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="AO1:AP1"/>
+    <mergeCell ref="AR1:AS1"/>
+    <mergeCell ref="AU1:AV1"/>
+    <mergeCell ref="AX1:AY1"/>
+    <mergeCell ref="Z1:AA1"/>
+    <mergeCell ref="AC1:AD1"/>
+    <mergeCell ref="AF1:AG1"/>
+    <mergeCell ref="AI1:AJ1"/>
+    <mergeCell ref="AL1:AM1"/>
     <mergeCell ref="BA1:BB1"/>
     <mergeCell ref="BD1:BE1"/>
     <mergeCell ref="A39:B39"/>
@@ -4495,15 +4526,6 @@
     <mergeCell ref="Q1:R1"/>
     <mergeCell ref="T1:U1"/>
     <mergeCell ref="W1:X1"/>
-    <mergeCell ref="AO1:AP1"/>
-    <mergeCell ref="AR1:AS1"/>
-    <mergeCell ref="AU1:AV1"/>
-    <mergeCell ref="AX1:AY1"/>
-    <mergeCell ref="Z1:AA1"/>
-    <mergeCell ref="AC1:AD1"/>
-    <mergeCell ref="AF1:AG1"/>
-    <mergeCell ref="AI1:AJ1"/>
-    <mergeCell ref="AL1:AM1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A40" r:id="rId1" xr:uid="{BD8505B1-6312-437D-81B2-778CAED7521D}"/>
@@ -4517,7 +4539,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96129535-FEF3-45F0-8A22-F7741A343589}">
   <dimension ref="A1:U42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
@@ -4532,30 +4554,30 @@
       </c>
       <c r="B1" s="17"/>
       <c r="D1" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E1" s="16"/>
       <c r="F1" s="10"/>
       <c r="G1" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H1" s="16"/>
       <c r="J1" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K1" s="16"/>
       <c r="L1" s="10"/>
       <c r="M1" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N1" s="16"/>
       <c r="P1" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q1" s="17"/>
       <c r="R1" s="10"/>
       <c r="S1" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="T1" s="17"/>
     </row>
@@ -4578,7 +4600,7 @@
         <v>15</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>15</v>
@@ -4591,7 +4613,7 @@
         <v>15</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P3" s="2" t="s">
         <v>15</v>
@@ -4604,7 +4626,7 @@
         <v>15</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.35">
@@ -5024,7 +5046,7 @@
       <c r="B41" s="16"/>
       <c r="C41" s="11"/>
       <c r="D41" s="17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E41" s="17"/>
       <c r="F41" s="17"/>
@@ -5096,23 +5118,23 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B1" s="16"/>
       <c r="D1" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E1" s="16"/>
       <c r="G1" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H1" s="16"/>
       <c r="J1" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K1" s="16"/>
       <c r="M1" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N1" s="16"/>
     </row>
@@ -5121,31 +5143,31 @@
         <v>15</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
@@ -5544,14 +5566,14 @@
     </row>
     <row r="36" spans="1:14" ht="79.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B36" s="16"/>
       <c r="C36" s="16"/>
       <c r="D36" s="16"/>
       <c r="E36" s="16"/>
       <c r="G36" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H36" s="16"/>
       <c r="I36" s="16"/>
@@ -6915,7 +6937,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I44" sqref="I44"/>
+      <selection activeCell="Q43" sqref="Q43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6929,7 +6951,7 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7056,7 +7078,7 @@
   <dimension ref="A1:Y65"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D47" sqref="D47:E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7083,7 +7105,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>31</v>
@@ -8377,10 +8399,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1076AE9C-2C87-4A85-AE97-8A00D25B1C89}">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8389,97 +8411,213 @@
     <col min="2" max="16384" width="9.1796875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="D1" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="5">
+        <v>374.76697420604501</v>
+      </c>
+      <c r="B4" s="5">
+        <v>215.90017889986299</v>
+      </c>
+      <c r="D4" s="5">
+        <v>375.65430566758101</v>
+      </c>
+      <c r="E4" s="5">
+        <v>83.230300780628596</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="5">
+        <v>412.10995015364199</v>
+      </c>
+      <c r="B5" s="5">
+        <v>215.87680469772599</v>
+      </c>
+      <c r="D5" s="5">
+        <v>412.45324706043198</v>
+      </c>
+      <c r="E5" s="5">
+        <v>81.215235235179406</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="5">
+        <v>474.554014292452</v>
+      </c>
+      <c r="B6" s="5">
+        <v>212.84967108660001</v>
+      </c>
+      <c r="D6" s="5">
+        <v>474.310642099799</v>
+      </c>
+      <c r="E6" s="5">
+        <v>82.570938959143305</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="5">
+        <v>540.89825105148998</v>
+      </c>
+      <c r="B7" s="5">
+        <v>210.01929941585399</v>
+      </c>
+      <c r="D7" s="5">
+        <v>541.76559757019902</v>
+      </c>
+      <c r="E7" s="5">
+        <v>80.337481614620103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="5">
+        <v>603.34231519030095</v>
+      </c>
+      <c r="B8" s="5">
+        <v>206.99216580472799</v>
+      </c>
+      <c r="D8" s="5">
+        <v>601.96823934345696</v>
+      </c>
+      <c r="E8" s="5">
+        <v>79.104579669049201</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="5">
+        <v>668.56250994275695</v>
+      </c>
+      <c r="B9" s="5">
+        <v>205.55692001976001</v>
+      </c>
+      <c r="D9" s="5">
+        <v>668.859175316284</v>
+      </c>
+      <c r="E9" s="5">
+        <v>77.867491299214905</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="5">
+        <v>732.68797393811303</v>
+      </c>
+      <c r="B10" s="5">
+        <v>201.13431165416799</v>
+      </c>
+      <c r="D10" s="5">
+        <v>729.06981106667297</v>
+      </c>
+      <c r="E10" s="5">
+        <v>75.439365226443698</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="5">
+        <v>793.45330287942204</v>
+      </c>
+      <c r="B11" s="5">
+        <v>199.104244755108</v>
+      </c>
+      <c r="D11" s="5">
+        <v>793.71532768538202</v>
+      </c>
+      <c r="E11" s="5">
+        <v>76.5941205857645</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="5">
+        <v>858.12146910000195</v>
+      </c>
+      <c r="B12" s="5">
+        <v>196.87253175402799</v>
+      </c>
+      <c r="D12" s="5">
+        <v>857.25678724033696</v>
+      </c>
+      <c r="E12" s="5">
+        <v>76.1559415128621</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D13" s="5">
+        <v>920.80490844290102</v>
+      </c>
+      <c r="E13" s="5">
+        <v>74.721742333959497</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D14" s="5">
+        <v>979.91015480001397</v>
+      </c>
+      <c r="E14" s="5">
+        <v>70.899885850165106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D15" s="5">
+        <v>1044.5743240320301</v>
+      </c>
+      <c r="E15" s="5">
+        <v>69.265784912685106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D16" s="5">
+        <v>1108.68380007312</v>
+      </c>
+      <c r="E16" s="5">
+        <v>67.233624801493704</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D17" s="5">
+        <v>1172.2532385480399</v>
+      </c>
+      <c r="E17" s="5">
+        <v>62.612161283390201</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D18" s="5">
+        <v>1232.4625419689</v>
+      </c>
+      <c r="E18" s="5">
+        <v>60.383239231819097</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="179.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="19"/>
-    </row>
-    <row r="3" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="5">
-        <v>17.541148288385699</v>
-      </c>
-      <c r="B4" s="5">
-        <v>33.767998351492601</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="5">
-        <v>147.82474306467799</v>
-      </c>
-      <c r="B5" s="5">
-        <v>32.228318264945997</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="5">
-        <v>297.73587821652097</v>
-      </c>
-      <c r="B6" s="5">
-        <v>36.684439636298002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="5">
-        <v>447.708832393168</v>
-      </c>
-      <c r="B7" s="5">
-        <v>40.214563531926899</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="5">
-        <v>498.24588517116098</v>
-      </c>
-      <c r="B8" s="5">
-        <v>33.211627128248601</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="5">
-        <v>548.53566184993394</v>
-      </c>
-      <c r="B9" s="5">
-        <v>29.912680627463001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="5">
-        <v>599.16544316513398</v>
-      </c>
-      <c r="B10" s="5">
-        <v>21.520748010200101</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="5">
-        <v>648.18792983540595</v>
-      </c>
-      <c r="B11" s="5">
-        <v>20.538083095072398</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="5">
-        <v>698.81771115060599</v>
-      </c>
-      <c r="B12" s="5">
-        <v>12.1461504778094</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="179.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="16" t="s">
-        <v>68</v>
-      </c>
       <c r="B27" s="16"/>
+    </row>
+    <row r="31" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+      <c r="A31" s="5" t="s">
+        <v>104</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -8517,19 +8655,19 @@
   <sheetData>
     <row r="1" spans="1:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B1" s="16"/>
       <c r="D1" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E1" s="16"/>
       <c r="G1" s="16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H1" s="16"/>
       <c r="J1" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K1" s="16"/>
     </row>
@@ -8548,28 +8686,28 @@
     </row>
     <row r="3" spans="1:11" ht="33.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="D3" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="G3" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="J3" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
@@ -8838,7 +8976,7 @@
     </row>
     <row r="36" spans="1:11" ht="53.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B36" s="16"/>
       <c r="C36" s="16"/>

</xml_diff>

<commit_message>
changes in Utilities package version 1.1
</commit_message>
<xml_diff>
--- a/Jupyter/Eurofer/Eurofer_data.xlsx
+++ b/Jupyter/Eurofer/Eurofer_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Research\Repos\DatabaseCodes\Jupyter\Eurofer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3EF6040-A6A6-4E59-8880-80E92C0A309F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE960FC-5A51-41A2-A04B-A32BE0C804C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="852" activeTab="2" xr2:uid="{D289EE42-B074-4616-9B9B-4CE9F1662138}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="852" activeTab="8" xr2:uid="{D289EE42-B074-4616-9B9B-4CE9F1662138}"/>
   </bookViews>
   <sheets>
     <sheet name="Density" sheetId="15" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="114">
   <si>
     <t>Temp (K)</t>
   </si>
@@ -200,12 +200,6 @@
   </si>
   <si>
     <t>Echaniz Eurofer Emissivity</t>
-  </si>
-  <si>
-    <t>EUROFER97 - As-rolled</t>
-  </si>
-  <si>
-    <t>EUROFER97 - Polished</t>
   </si>
   <si>
     <t>Hemispherical Emissivity</t>
@@ -340,9 +334,6 @@
     </r>
   </si>
   <si>
-    <t>EUROFER97 - polished</t>
-  </si>
-  <si>
     <t>Coefficient of Thermal Expansion</t>
   </si>
   <si>
@@ -558,18 +549,6 @@
     <t>Schäfer, Ludwig, and Helmut Kempe. Zug-und Kerbschlageigenschaften des Stahles EUROFER'97 (Vergleich mit OPTIFER). Forschungszentrum Karlsruhe, 2000.</t>
   </si>
   <si>
-    <t>Eurofer97 Heat 993391_1040 C</t>
-  </si>
-  <si>
-    <t>Eurofer97 Heat 993402_1040 C</t>
-  </si>
-  <si>
-    <t>Eurofer97 Heat 993391_980 C</t>
-  </si>
-  <si>
-    <t>Eurofer97 Heat 993402_980 C</t>
-  </si>
-  <si>
     <t>T [°C]</t>
   </si>
   <si>
@@ -667,6 +646,33 @@
   </si>
   <si>
     <t>Mergia2008</t>
+  </si>
+  <si>
+    <t>Echaniz2021 - As-rolled</t>
+  </si>
+  <si>
+    <t>Echaniz2021 - Polished</t>
+  </si>
+  <si>
+    <t>Echaniz2021 - polished</t>
+  </si>
+  <si>
+    <t>Echaniz2021</t>
+  </si>
+  <si>
+    <t>Tavassoli2002</t>
+  </si>
+  <si>
+    <t>Schaefer2000-Heat 993391_1040 C</t>
+  </si>
+  <si>
+    <t>Schaefer2000- Heat 993402_1040 C</t>
+  </si>
+  <si>
+    <t>Schaefer2000- Heat 993391_980 C</t>
+  </si>
+  <si>
+    <t>Schaefer2000-Heat 993402_980 C</t>
   </si>
 </sst>
 </file>
@@ -779,7 +785,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -824,6 +830,9 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -839,8 +848,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2600,17 +2609,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="16"/>
+      <c r="B1" s="17"/>
     </row>
     <row r="3" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -2670,20 +2679,20 @@
       </c>
     </row>
     <row r="45" spans="1:3" ht="217.5" x14ac:dyDescent="0.35">
-      <c r="A45" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="B45" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="C45" s="21" t="s">
-        <v>92</v>
+      <c r="A45" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B45" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C45" s="16" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A46" s="21"/>
-      <c r="B46" s="21"/>
-      <c r="C46" s="21"/>
+      <c r="A46" s="16"/>
+      <c r="B46" s="16"/>
+      <c r="C46" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2729,67 +2738,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16" t="s">
+      <c r="J1" s="17"/>
+      <c r="K1" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16" t="s">
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="T1" s="16"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="T1" s="17"/>
       <c r="U1" s="11"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="17"/>
       <c r="AA1" s="11"/>
-      <c r="AB1" s="16"/>
-      <c r="AC1" s="16"/>
+      <c r="AB1" s="17"/>
+      <c r="AC1" s="17"/>
       <c r="AG1" s="11"/>
-      <c r="AH1" s="16"/>
-      <c r="AI1" s="16"/>
+      <c r="AH1" s="17"/>
+      <c r="AI1" s="17"/>
       <c r="AM1" s="11"/>
-      <c r="AN1" s="16"/>
-      <c r="AO1" s="16"/>
+      <c r="AN1" s="17"/>
+      <c r="AO1" s="17"/>
       <c r="AS1" s="11"/>
-      <c r="AT1" s="16"/>
-      <c r="AU1" s="16"/>
+      <c r="AT1" s="17"/>
+      <c r="AU1" s="17"/>
       <c r="AY1" s="11"/>
-      <c r="AZ1" s="16"/>
-      <c r="BA1" s="16"/>
+      <c r="AZ1" s="17"/>
+      <c r="BA1" s="17"/>
     </row>
     <row r="2" spans="1:53" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:53" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:53" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -2809,7 +2818,7 @@
         <v>16</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>16</v>
@@ -3453,73 +3462,73 @@
     </row>
     <row r="23" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:53" ht="152.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="16" t="s">
+      <c r="A25" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="16"/>
+      <c r="B25" s="17"/>
       <c r="C25" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="16"/>
-      <c r="K25" s="16"/>
-      <c r="L25" s="16"/>
-      <c r="M25" s="16"/>
-      <c r="N25" s="16"/>
-      <c r="O25" s="16"/>
-      <c r="P25" s="16"/>
-      <c r="Q25" s="16"/>
-      <c r="R25" s="16"/>
-      <c r="S25" s="16"/>
-      <c r="T25" s="16"/>
-      <c r="U25" s="16"/>
-      <c r="V25" s="16"/>
-      <c r="W25" s="16"/>
-      <c r="X25" s="16"/>
-      <c r="Y25" s="16"/>
-      <c r="Z25" s="16"/>
-      <c r="AA25" s="16"/>
-      <c r="AB25" s="16"/>
-      <c r="AC25" s="16"/>
-      <c r="AD25" s="16"/>
-      <c r="AE25" s="16"/>
-      <c r="AF25" s="16"/>
-      <c r="AG25" s="16"/>
-      <c r="AH25" s="16"/>
-      <c r="AI25" s="16"/>
-      <c r="AJ25" s="16"/>
-      <c r="AK25" s="16"/>
-      <c r="AL25" s="16"/>
-      <c r="AM25" s="16"/>
-      <c r="AN25" s="16"/>
-      <c r="AO25" s="16"/>
-      <c r="AP25" s="16"/>
-      <c r="AQ25" s="16"/>
-      <c r="AR25" s="16"/>
-      <c r="AS25" s="16"/>
-      <c r="AT25" s="16"/>
-      <c r="AU25" s="16"/>
-      <c r="AV25" s="16"/>
-      <c r="AW25" s="16"/>
-      <c r="AX25" s="16"/>
-      <c r="AY25" s="16"/>
-      <c r="AZ25" s="16"/>
-      <c r="BA25" s="16"/>
+        <v>50</v>
+      </c>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17"/>
+      <c r="K25" s="17"/>
+      <c r="L25" s="17"/>
+      <c r="M25" s="17"/>
+      <c r="N25" s="17"/>
+      <c r="O25" s="17"/>
+      <c r="P25" s="17"/>
+      <c r="Q25" s="17"/>
+      <c r="R25" s="17"/>
+      <c r="S25" s="17"/>
+      <c r="T25" s="17"/>
+      <c r="U25" s="17"/>
+      <c r="V25" s="17"/>
+      <c r="W25" s="17"/>
+      <c r="X25" s="17"/>
+      <c r="Y25" s="17"/>
+      <c r="Z25" s="17"/>
+      <c r="AA25" s="17"/>
+      <c r="AB25" s="17"/>
+      <c r="AC25" s="17"/>
+      <c r="AD25" s="17"/>
+      <c r="AE25" s="17"/>
+      <c r="AF25" s="17"/>
+      <c r="AG25" s="17"/>
+      <c r="AH25" s="17"/>
+      <c r="AI25" s="17"/>
+      <c r="AJ25" s="17"/>
+      <c r="AK25" s="17"/>
+      <c r="AL25" s="17"/>
+      <c r="AM25" s="17"/>
+      <c r="AN25" s="17"/>
+      <c r="AO25" s="17"/>
+      <c r="AP25" s="17"/>
+      <c r="AQ25" s="17"/>
+      <c r="AR25" s="17"/>
+      <c r="AS25" s="17"/>
+      <c r="AT25" s="17"/>
+      <c r="AU25" s="17"/>
+      <c r="AV25" s="17"/>
+      <c r="AW25" s="17"/>
+      <c r="AX25" s="17"/>
+      <c r="AY25" s="17"/>
+      <c r="AZ25" s="17"/>
+      <c r="BA25" s="17"/>
     </row>
     <row r="26" spans="1:53" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
@@ -3528,14 +3537,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="AZ1:BA1"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="G25:J25"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
     <mergeCell ref="K25:BA25"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="O1:P1"/>
@@ -3544,9 +3545,17 @@
     <mergeCell ref="AT1:AU1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="K1:L1"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="G25:J25"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
     <mergeCell ref="AB1:AC1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="AH1:AI1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="AZ1:BA1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A26" r:id="rId1" xr:uid="{BD8505B1-6312-437D-81B2-778CAED7521D}"/>
@@ -3574,42 +3583,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16" t="s">
+      <c r="F1" s="17"/>
+      <c r="G1" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="R1" s="16"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="R1" s="17"/>
     </row>
     <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:18" ht="58" x14ac:dyDescent="0.35">
@@ -3617,55 +3626,55 @@
         <v>15</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="Q3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
@@ -4037,17 +4046,16 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="G21" s="7" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B22" s="7" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="O1:P1"/>
     <mergeCell ref="Q1:R1"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="K1:L1"/>
@@ -4056,6 +4064,7 @@
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="O1:P1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B22" r:id="rId1" xr:uid="{49CE8F48-BC1C-42DF-8D69-1569F2C329D5}"/>
@@ -4094,37 +4103,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="D1" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="D1" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="17"/>
       <c r="F1" s="10"/>
-      <c r="G1" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="H1" s="16"/>
-      <c r="J1" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="K1" s="16"/>
+      <c r="G1" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="17"/>
+      <c r="J1" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="K1" s="17"/>
       <c r="L1" s="10"/>
-      <c r="M1" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="N1" s="16"/>
-      <c r="P1" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q1" s="17"/>
+      <c r="M1" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="N1" s="17"/>
+      <c r="P1" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q1" s="18"/>
       <c r="R1" s="10"/>
-      <c r="S1" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="T1" s="17"/>
+      <c r="S1" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="T1" s="18"/>
     </row>
     <row r="3" spans="1:21" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
@@ -4145,7 +4154,7 @@
         <v>15</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>15</v>
@@ -4158,7 +4167,7 @@
         <v>15</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="P3" s="2" t="s">
         <v>15</v>
@@ -4171,7 +4180,7 @@
         <v>15</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.35">
@@ -4585,37 +4594,37 @@
       <c r="C18" s="6"/>
     </row>
     <row r="41" spans="1:21" ht="84.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="16" t="s">
+      <c r="A41" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B41" s="16"/>
+      <c r="B41" s="17"/>
       <c r="C41" s="11"/>
-      <c r="D41" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="E41" s="17"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="17"/>
-      <c r="H41" s="17"/>
-      <c r="I41" s="17"/>
-      <c r="J41" s="17"/>
-      <c r="K41" s="17"/>
-      <c r="L41" s="17"/>
-      <c r="M41" s="17"/>
-      <c r="N41" s="17"/>
-      <c r="O41" s="17"/>
-      <c r="P41" s="17"/>
-      <c r="Q41" s="17"/>
-      <c r="R41" s="17"/>
-      <c r="S41" s="17"/>
-      <c r="T41" s="17"/>
-      <c r="U41" s="17"/>
+      <c r="D41" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="18"/>
+      <c r="I41" s="18"/>
+      <c r="J41" s="18"/>
+      <c r="K41" s="18"/>
+      <c r="L41" s="18"/>
+      <c r="M41" s="18"/>
+      <c r="N41" s="18"/>
+      <c r="O41" s="18"/>
+      <c r="P41" s="18"/>
+      <c r="Q41" s="18"/>
+      <c r="R41" s="18"/>
+      <c r="S41" s="18"/>
+      <c r="T41" s="18"/>
+      <c r="U41" s="18"/>
     </row>
     <row r="42" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="20" t="s">
+      <c r="A42" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B42" s="20"/>
+      <c r="B42" s="21"/>
       <c r="C42" s="7"/>
     </row>
   </sheetData>
@@ -4662,57 +4671,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="D1" s="16" t="s">
+      <c r="A1" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="D1" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="17"/>
+      <c r="G1" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="G1" s="16" t="s">
+      <c r="H1" s="17"/>
+      <c r="J1" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="H1" s="16"/>
-      <c r="J1" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="K1" s="16"/>
-      <c r="M1" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="N1" s="16"/>
+      <c r="K1" s="17"/>
+      <c r="M1" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="N1" s="17"/>
     </row>
     <row r="3" spans="1:14" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
@@ -5110,23 +5119,23 @@
       </c>
     </row>
     <row r="36" spans="1:14" ht="79.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="B36" s="16"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
-      <c r="G36" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="H36" s="16"/>
-      <c r="I36" s="16"/>
-      <c r="J36" s="16"/>
-      <c r="K36" s="16"/>
-      <c r="L36" s="16"/>
-      <c r="M36" s="16"/>
-      <c r="N36" s="16"/>
+      <c r="A36" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
+      <c r="G36" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="H36" s="17"/>
+      <c r="I36" s="17"/>
+      <c r="J36" s="17"/>
+      <c r="K36" s="17"/>
+      <c r="L36" s="17"/>
+      <c r="M36" s="17"/>
+      <c r="N36" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -5171,57 +5180,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="D1" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="17"/>
+      <c r="G1" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="D1" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="16"/>
-      <c r="G1" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="H1" s="16"/>
-      <c r="J1" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="K1" s="16"/>
-      <c r="M1" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="N1" s="16"/>
+      <c r="H1" s="17"/>
+      <c r="J1" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" s="17"/>
+      <c r="M1" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="N1" s="17"/>
     </row>
     <row r="3" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
@@ -5545,36 +5554,36 @@
       </c>
     </row>
     <row r="32" spans="13:23" x14ac:dyDescent="0.35">
-      <c r="M32" s="16"/>
-      <c r="N32" s="16"/>
-      <c r="O32" s="16"/>
-      <c r="P32" s="16"/>
-      <c r="Q32" s="16"/>
-      <c r="R32" s="16"/>
-      <c r="S32" s="16"/>
-      <c r="T32" s="16"/>
-      <c r="U32" s="16"/>
-      <c r="V32" s="16"/>
-      <c r="W32" s="16"/>
+      <c r="M32" s="17"/>
+      <c r="N32" s="17"/>
+      <c r="O32" s="17"/>
+      <c r="P32" s="17"/>
+      <c r="Q32" s="17"/>
+      <c r="R32" s="17"/>
+      <c r="S32" s="17"/>
+      <c r="T32" s="17"/>
+      <c r="U32" s="17"/>
+      <c r="V32" s="17"/>
+      <c r="W32" s="17"/>
     </row>
     <row r="34" spans="1:23" ht="147" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="B34" s="16"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="16"/>
-      <c r="I34" s="16"/>
-      <c r="J34" s="16"/>
-      <c r="K34" s="16"/>
-      <c r="M34" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="N34" s="16"/>
+      <c r="A34" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="17"/>
+      <c r="J34" s="17"/>
+      <c r="K34" s="17"/>
+      <c r="M34" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="N34" s="17"/>
       <c r="O34" s="11"/>
       <c r="P34" s="11"/>
       <c r="Q34" s="11"/>
@@ -5629,77 +5638,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="D1" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="D1" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" s="16"/>
-      <c r="G1" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="H1" s="16"/>
-      <c r="J1" s="16" t="s">
+      <c r="E1" s="17"/>
+      <c r="G1" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="K1" s="16"/>
-      <c r="M1" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="N1" s="16"/>
-      <c r="P1" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q1" s="16"/>
-      <c r="S1" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="T1" s="16"/>
+      <c r="H1" s="17"/>
+      <c r="J1" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" s="17"/>
+      <c r="M1" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" s="17"/>
+      <c r="P1" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q1" s="17"/>
+      <c r="S1" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="T1" s="17"/>
     </row>
     <row r="3" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.35">
@@ -6431,32 +6440,32 @@
       </c>
     </row>
     <row r="39" spans="1:17" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B39" s="16"/>
-      <c r="C39" s="16"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="16"/>
-      <c r="G39" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="H39" s="16"/>
-      <c r="I39" s="16"/>
-      <c r="J39" s="16"/>
-      <c r="K39" s="16"/>
-      <c r="L39" s="16"/>
-      <c r="M39" s="16"/>
-      <c r="N39" s="16"/>
+      <c r="A39" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
+      <c r="G39" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="H39" s="17"/>
+      <c r="I39" s="17"/>
+      <c r="J39" s="17"/>
+      <c r="K39" s="17"/>
+      <c r="L39" s="17"/>
+      <c r="M39" s="17"/>
+      <c r="N39" s="17"/>
     </row>
     <row r="52" spans="16:20" ht="93.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="P52" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q52" s="16"/>
-      <c r="R52" s="16"/>
-      <c r="S52" s="16"/>
-      <c r="T52" s="16"/>
+      <c r="P52" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q52" s="17"/>
+      <c r="R52" s="17"/>
+      <c r="S52" s="17"/>
+      <c r="T52" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -6506,12 +6515,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
+      <c r="B1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -6593,10 +6602,10 @@
       </c>
     </row>
     <row r="36" spans="1:2" ht="156" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="16" t="s">
+      <c r="A36" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="16"/>
+      <c r="B36" s="17"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="12" t="s">
@@ -6622,8 +6631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{234A6B1F-5943-445E-8C13-06397E85A588}">
   <dimension ref="A1:Y65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6633,14 +6642,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="D1" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="E1" s="16"/>
+      <c r="A1" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="D1" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" s="17"/>
     </row>
     <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
@@ -6650,10 +6659,10 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -6957,26 +6966,26 @@
       <c r="Y36" s="7"/>
     </row>
     <row r="47" spans="1:25" ht="285" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="16" t="s">
+      <c r="A47" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B47" s="16"/>
-      <c r="D47" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="E47" s="16"/>
+      <c r="B47" s="17"/>
+      <c r="D47" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E47" s="17"/>
     </row>
     <row r="49" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A49" s="7" t="s">
         <v>5</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F50" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.35">
@@ -7074,8 +7083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D45C8D-0E1D-4271-9C84-7C91BB3EB92B}">
   <dimension ref="A1:V49"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7085,14 +7094,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="D1" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="16"/>
+      <c r="A1" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="D1" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" s="17"/>
     </row>
     <row r="3" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
@@ -7105,7 +7114,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -7274,23 +7283,26 @@
       </c>
     </row>
     <row r="33" spans="1:22" ht="208.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="16" t="s">
+      <c r="A33" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B33" s="16"/>
-      <c r="D33" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="E33" s="16"/>
+      <c r="B33" s="17"/>
+      <c r="D33" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E33" s="17"/>
     </row>
     <row r="35" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="7" t="s">
         <v>5</v>
       </c>
+      <c r="F35" s="7" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.35">
       <c r="D36" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.35">
@@ -7368,9 +7380,10 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A35" r:id="rId1" xr:uid="{7FC28E87-51CA-4509-BEAB-A0CCB56EBA75}"/>
+    <hyperlink ref="F35" r:id="rId2" xr:uid="{29F717C2-C836-48B4-A652-F7CA04355D78}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -7393,14 +7406,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="D1" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="E1" s="17"/>
+      <c r="B1" s="18"/>
+      <c r="D1" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="E1" s="18"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -7416,7 +7429,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>4</v>
@@ -7430,11 +7443,11 @@
         <v>51.077844311377198</v>
       </c>
       <c r="D4" s="10">
-        <f>D29+273</f>
+        <f t="shared" ref="D4:D17" si="0">D29+273</f>
         <v>293</v>
       </c>
       <c r="E4" s="10">
-        <f>E29*100</f>
+        <f t="shared" ref="E4:E17" si="1">E29*100</f>
         <v>50</v>
       </c>
     </row>
@@ -7446,11 +7459,11 @@
         <v>54.550898203592801</v>
       </c>
       <c r="D5" s="10">
-        <f>D30+273</f>
+        <f t="shared" si="0"/>
         <v>323</v>
       </c>
       <c r="E5" s="10">
-        <f>E30*100</f>
+        <f t="shared" si="1"/>
         <v>54</v>
       </c>
     </row>
@@ -7462,11 +7475,11 @@
         <v>56.467065868263397</v>
       </c>
       <c r="D6" s="10">
-        <f>D31+273</f>
+        <f t="shared" si="0"/>
         <v>373</v>
       </c>
       <c r="E6" s="10">
-        <f>E31*100</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
     </row>
@@ -7478,11 +7491,11 @@
         <v>59.101796407185603</v>
       </c>
       <c r="D7" s="10">
-        <f>D32+273</f>
+        <f t="shared" si="0"/>
         <v>423</v>
       </c>
       <c r="E7" s="10">
-        <f>E32*100</f>
+        <f t="shared" si="1"/>
         <v>67</v>
       </c>
     </row>
@@ -7494,11 +7507,11 @@
         <v>62.814371257485</v>
       </c>
       <c r="D8" s="10">
-        <f>D33+273</f>
+        <f t="shared" si="0"/>
         <v>473</v>
       </c>
       <c r="E8" s="10">
-        <f>E33*100</f>
+        <f t="shared" si="1"/>
         <v>74</v>
       </c>
     </row>
@@ -7510,11 +7523,11 @@
         <v>66.407185628742496</v>
       </c>
       <c r="D9" s="10">
-        <f>D34+273</f>
+        <f t="shared" si="0"/>
         <v>523</v>
       </c>
       <c r="E9" s="10">
-        <f>E34*100</f>
+        <f t="shared" si="1"/>
         <v>80</v>
       </c>
     </row>
@@ -7526,11 +7539,11 @@
         <v>69.281437125748496</v>
       </c>
       <c r="D10" s="10">
-        <f>D35+273</f>
+        <f t="shared" si="0"/>
         <v>573</v>
       </c>
       <c r="E10" s="10">
-        <f>E35*100</f>
+        <f t="shared" si="1"/>
         <v>87</v>
       </c>
     </row>
@@ -7542,11 +7555,11 @@
         <v>71.437125748502893</v>
       </c>
       <c r="D11" s="10">
-        <f>D36+273</f>
+        <f t="shared" si="0"/>
         <v>623</v>
       </c>
       <c r="E11" s="10">
-        <f>E36*100</f>
+        <f t="shared" si="1"/>
         <v>93</v>
       </c>
     </row>
@@ -7558,11 +7571,11 @@
         <v>75.508982035928099</v>
       </c>
       <c r="D12" s="10">
-        <f>D37+273</f>
+        <f t="shared" si="0"/>
         <v>673</v>
       </c>
       <c r="E12" s="10">
-        <f>E37*100</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
@@ -7574,11 +7587,11 @@
         <v>77.425149700598794</v>
       </c>
       <c r="D13" s="10">
-        <f>D38+273</f>
+        <f t="shared" si="0"/>
         <v>723</v>
       </c>
       <c r="E13" s="10">
-        <f>E38*100</f>
+        <f t="shared" si="1"/>
         <v>107</v>
       </c>
     </row>
@@ -7590,11 +7603,11 @@
         <v>81.137724550898199</v>
       </c>
       <c r="D14" s="10">
-        <f>D39+273</f>
+        <f t="shared" si="0"/>
         <v>773</v>
       </c>
       <c r="E14" s="10">
-        <f>E39*100</f>
+        <f t="shared" si="1"/>
         <v>112.99999999999999</v>
       </c>
     </row>
@@ -7606,11 +7619,11 @@
         <v>84.730538922155603</v>
       </c>
       <c r="D15" s="10">
-        <f>D40+273</f>
+        <f t="shared" si="0"/>
         <v>823</v>
       </c>
       <c r="E15" s="10">
-        <f>E40*100</f>
+        <f t="shared" si="1"/>
         <v>120</v>
       </c>
     </row>
@@ -7622,11 +7635,11 @@
         <v>87.245508982035901</v>
       </c>
       <c r="D16" s="10">
-        <f>D41+273</f>
+        <f t="shared" si="0"/>
         <v>873</v>
       </c>
       <c r="E16" s="10">
-        <f>E41*100</f>
+        <f t="shared" si="1"/>
         <v>127</v>
       </c>
     </row>
@@ -7638,11 +7651,11 @@
         <v>93.473053892215503</v>
       </c>
       <c r="D17" s="10">
-        <f>D42+273</f>
+        <f t="shared" si="0"/>
         <v>923</v>
       </c>
       <c r="E17" s="10">
-        <f>E42*100</f>
+        <f t="shared" si="1"/>
         <v>133</v>
       </c>
     </row>
@@ -7720,10 +7733,10 @@
     </row>
     <row r="28" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="D28" s="5" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -7840,26 +7853,26 @@
       </c>
     </row>
     <row r="45" spans="2:22" ht="232" x14ac:dyDescent="0.35">
-      <c r="D45" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="E45" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="F45" s="21" t="s">
-        <v>92</v>
+      <c r="D45" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="E45" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F45" s="16" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="46" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B46" s="12" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="210" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="16" t="s">
+      <c r="A53" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B53" s="16"/>
+      <c r="B53" s="17"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="12" t="s">
@@ -7895,17 +7908,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="16"/>
+      <c r="B1" s="17"/>
     </row>
     <row r="3" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -7965,10 +7978,10 @@
       </c>
     </row>
     <row r="39" spans="1:2" ht="187.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="16" t="s">
+      <c r="A39" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B39" s="16"/>
+      <c r="B39" s="17"/>
     </row>
     <row r="40" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" s="7" t="s">
@@ -7990,10 +8003,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B73F6F46-AAA6-4839-9EF2-18966D033E04}">
-  <dimension ref="A1:N34"/>
+  <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:H1"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8002,18 +8015,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="D1" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="16"/>
-      <c r="G1" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1" s="16"/>
+      <c r="A1" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="D1" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" s="17"/>
+      <c r="G1" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="H1" s="17"/>
       <c r="I1" s="11"/>
     </row>
     <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -8021,19 +8034,19 @@
         <v>0</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -8156,30 +8169,35 @@
       <c r="M32" s="9"/>
     </row>
     <row r="33" spans="1:14" ht="153" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="18" t="s">
+      <c r="A33" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" s="19"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="B33" s="18"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
-      <c r="H33" s="18"/>
-      <c r="I33" s="18"/>
-      <c r="J33" s="9"/>
-      <c r="K33" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="L33" s="18"/>
-      <c r="M33" s="18"/>
-      <c r="N33" s="18"/>
+      <c r="L33" s="19"/>
+      <c r="M33" s="19"/>
+      <c r="N33" s="19"/>
     </row>
     <row r="34" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A34" s="9" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E35" s="7" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -8193,9 +8211,10 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A34" r:id="rId1" xr:uid="{BA9D3B74-4905-46E0-83D8-53DCA582D837}"/>
+    <hyperlink ref="E35" r:id="rId2" xr:uid="{E1B57220-379F-400D-AEB2-773015CA6E3F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -8204,7 +8223,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8214,26 +8233,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="B1" s="19"/>
+      <c r="A1" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="20"/>
       <c r="D1" s="5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -8411,14 +8430,19 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="179.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="B27" s="16"/>
+      <c r="A27" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" s="17"/>
+    </row>
+    <row r="30" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="C30" s="22" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="31" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -8426,8 +8450,11 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A27:B27"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C30" r:id="rId1" xr:uid="{20C01742-4F6F-4C19-B5CF-C6258268DDFB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -8435,8 +8462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22B499B7-5D41-461D-8465-819EE01970F8}">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8456,22 +8483,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="D1" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="E1" s="16"/>
-      <c r="G1" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="H1" s="16"/>
-      <c r="J1" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="K1" s="16"/>
+      <c r="A1" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="D1" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" s="17"/>
+      <c r="G1" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="H1" s="17"/>
+      <c r="J1" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="K1" s="17"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
@@ -8488,28 +8515,28 @@
     </row>
     <row r="3" spans="1:11" ht="33.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
@@ -8849,23 +8876,23 @@
       </c>
     </row>
     <row r="39" spans="1:11" ht="53.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="B39" s="16"/>
-      <c r="C39" s="16"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="16"/>
-      <c r="G39" s="16"/>
-      <c r="H39" s="16"/>
-      <c r="I39" s="16"/>
-      <c r="J39" s="16"/>
-      <c r="K39" s="16"/>
+      <c r="A39" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="17"/>
+      <c r="H39" s="17"/>
+      <c r="I39" s="17"/>
+      <c r="J39" s="17"/>
+      <c r="K39" s="17"/>
     </row>
     <row r="41" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="B41" s="7" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>